<commit_message>
ajout des codes de couleur
</commit_message>
<xml_diff>
--- a/datas_lab_IN.xlsx
+++ b/datas_lab_IN.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
+    <workbookView xWindow="14460" yWindow="0" windowWidth="11140" windowHeight="14540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,15 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="5">
   <si>
     <t>Temperature</t>
   </si>
   <si>
     <t>Nb frozen</t>
-  </si>
-  <si>
-    <t>Code</t>
   </si>
   <si>
     <t>Temperature [°C]</t>
@@ -36,14 +33,14 @@
     <t/>
   </si>
   <si>
-    <t>code</t>
+    <t>[Month, Source]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -55,6 +52,18 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -75,8 +84,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -85,7 +96,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -417,8 +430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CU32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
-      <selection activeCell="BQ4" sqref="BQ4"/>
+    <sheetView tabSelected="1" topLeftCell="BI2" workbookViewId="0">
+      <selection activeCell="BQ5" sqref="BQ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -616,7 +629,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>0</v>
@@ -624,148 +637,197 @@
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="I2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="J2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="L2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="M2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="N2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="O2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="P2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="R2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="S2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="U2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="V2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="X2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="Y2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AA2" s="1"/>
+      <c r="AA2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AB2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AD2" s="1"/>
+      <c r="AD2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AE2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AG2" s="1"/>
+      <c r="AG2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AH2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AI2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AJ2" s="1"/>
+      <c r="AJ2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AK2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AL2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AM2" s="1"/>
+      <c r="AM2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AN2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AO2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AP2" s="1"/>
+      <c r="AP2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AQ2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AR2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AS2" s="1"/>
+      <c r="AS2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AT2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AU2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AV2" s="1"/>
+      <c r="AV2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AW2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AX2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="AY2" s="1"/>
+      <c r="AY2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="AZ2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BA2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BB2" s="1"/>
+      <c r="BB2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="BC2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BD2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BE2" s="1"/>
+      <c r="BE2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="BF2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BG2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BH2" s="1"/>
+      <c r="BH2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="BI2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BJ2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BK2" s="1"/>
+      <c r="BK2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="BL2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BM2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="BN2" s="1"/>
+      <c r="BN2" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="BO2" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="BP2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="BR2" s="1"/>
       <c r="BS2" s="1"/>
@@ -805,24 +867,36 @@
       <c r="B3" s="1">
         <v>0</v>
       </c>
+      <c r="C3">
+        <v>11</v>
+      </c>
       <c r="D3" s="1">
         <v>-1</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
       </c>
+      <c r="F3">
+        <v>11</v>
+      </c>
       <c r="G3" s="1">
         <v>-1</v>
       </c>
       <c r="H3" s="1">
         <v>0</v>
       </c>
+      <c r="I3">
+        <v>10</v>
+      </c>
       <c r="J3" s="1">
         <v>-1</v>
       </c>
       <c r="K3" s="1">
         <v>0</v>
       </c>
+      <c r="L3">
+        <v>10</v>
+      </c>
       <c r="M3" s="1">
         <v>-1</v>
       </c>
@@ -835,124 +909,158 @@
       <c r="Q3" s="1">
         <v>0</v>
       </c>
+      <c r="R3">
+        <v>9</v>
+      </c>
       <c r="S3" s="1">
         <v>-1</v>
       </c>
       <c r="T3" s="1">
         <v>0</v>
       </c>
+      <c r="U3">
+        <v>9</v>
+      </c>
       <c r="V3" s="1">
         <v>-1</v>
       </c>
       <c r="W3" s="1">
         <v>0</v>
       </c>
+      <c r="X3">
+        <v>11</v>
+      </c>
       <c r="Y3" s="1">
         <v>-1</v>
       </c>
       <c r="Z3" s="1">
         <v>0</v>
       </c>
-      <c r="AA3" s="1"/>
+      <c r="AA3">
+        <v>11</v>
+      </c>
       <c r="AB3" s="1">
         <v>-1</v>
       </c>
       <c r="AC3" s="1">
         <v>0</v>
       </c>
-      <c r="AD3" s="1"/>
+      <c r="AD3">
+        <v>11</v>
+      </c>
       <c r="AE3" s="1">
         <v>-1</v>
       </c>
       <c r="AF3" s="1">
         <v>0</v>
       </c>
-      <c r="AG3" s="1"/>
+      <c r="AG3">
+        <v>10</v>
+      </c>
       <c r="AH3" s="1">
         <v>-1</v>
       </c>
       <c r="AI3" s="1">
         <v>0</v>
       </c>
-      <c r="AJ3" s="1"/>
+      <c r="AJ3">
+        <v>10</v>
+      </c>
       <c r="AK3" s="1">
         <v>-1</v>
       </c>
       <c r="AL3" s="1">
         <v>0</v>
       </c>
-      <c r="AM3" s="1"/>
+      <c r="AM3">
+        <v>10</v>
+      </c>
       <c r="AN3" s="1">
         <v>-1</v>
       </c>
       <c r="AO3" s="1">
         <v>0</v>
       </c>
-      <c r="AP3" s="1"/>
+      <c r="AP3">
+        <v>11</v>
+      </c>
       <c r="AQ3" s="1">
         <v>-1</v>
       </c>
       <c r="AR3" s="1">
         <v>0</v>
       </c>
-      <c r="AS3" s="1"/>
       <c r="AT3" s="1">
         <v>-1</v>
       </c>
       <c r="AU3" s="1">
         <v>0</v>
       </c>
-      <c r="AV3" s="1"/>
+      <c r="AV3">
+        <v>11</v>
+      </c>
       <c r="AW3" s="1">
         <v>-1</v>
       </c>
       <c r="AX3" s="1">
         <v>0</v>
       </c>
-      <c r="AY3" s="1"/>
+      <c r="AY3">
+        <v>11</v>
+      </c>
       <c r="AZ3" s="1">
         <v>-1</v>
       </c>
       <c r="BA3" s="1">
         <v>0</v>
       </c>
-      <c r="BB3" s="1"/>
+      <c r="BB3">
+        <v>12</v>
+      </c>
       <c r="BC3" s="1">
         <v>-1</v>
       </c>
       <c r="BD3" s="1">
         <v>0</v>
       </c>
-      <c r="BE3" s="1"/>
+      <c r="BE3">
+        <v>12</v>
+      </c>
       <c r="BF3" s="1">
         <v>-1</v>
       </c>
       <c r="BG3" s="1">
         <v>0</v>
       </c>
-      <c r="BH3" s="1"/>
+      <c r="BH3">
+        <v>12</v>
+      </c>
       <c r="BI3" s="1">
         <v>-1</v>
       </c>
       <c r="BJ3" s="1">
         <v>0</v>
       </c>
-      <c r="BK3" s="1"/>
+      <c r="BK3">
+        <v>12</v>
+      </c>
       <c r="BL3" s="1">
         <v>-1</v>
       </c>
       <c r="BM3" s="1">
         <v>0</v>
       </c>
-      <c r="BN3" s="1"/>
+      <c r="BN3">
+        <v>12</v>
+      </c>
       <c r="BO3" s="1">
         <v>-1</v>
       </c>
       <c r="BP3" s="1">
         <v>0</v>
       </c>
-      <c r="BQ3" s="1">
-        <v>0</v>
+      <c r="BQ3">
+        <v>12</v>
       </c>
       <c r="BR3" s="1"/>
       <c r="BS3" s="1"/>
@@ -992,24 +1100,36 @@
       <c r="B4" s="1">
         <v>0</v>
       </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
       <c r="D4" s="1">
         <v>-2</v>
       </c>
       <c r="E4" s="1">
         <v>0</v>
       </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
       <c r="G4" s="1">
         <v>-2</v>
       </c>
       <c r="H4" s="1">
         <v>0</v>
       </c>
+      <c r="I4" s="1">
+        <v>3</v>
+      </c>
       <c r="J4" s="1">
         <v>-2</v>
       </c>
       <c r="K4" s="1">
         <v>0</v>
       </c>
+      <c r="L4" s="1">
+        <v>1</v>
+      </c>
       <c r="M4" s="1">
         <v>-2</v>
       </c>
@@ -1022,60 +1142,81 @@
       <c r="Q4" s="1">
         <v>0</v>
       </c>
+      <c r="R4" s="1">
+        <v>2</v>
+      </c>
       <c r="S4" s="1">
         <v>-2</v>
       </c>
       <c r="T4" s="1">
         <v>0</v>
       </c>
+      <c r="U4" s="1">
+        <v>1</v>
+      </c>
       <c r="V4" s="1">
         <v>-2</v>
       </c>
       <c r="W4" s="1">
         <v>0</v>
       </c>
+      <c r="X4" s="1">
+        <v>2</v>
+      </c>
       <c r="Y4" s="1">
         <v>-2</v>
       </c>
       <c r="Z4" s="1">
         <v>0</v>
       </c>
-      <c r="AA4" s="1"/>
+      <c r="AA4" s="1">
+        <v>0</v>
+      </c>
       <c r="AB4" s="1">
         <v>-2</v>
       </c>
       <c r="AC4" s="1">
         <v>0</v>
       </c>
-      <c r="AD4" s="1"/>
+      <c r="AD4" s="1">
+        <v>0</v>
+      </c>
       <c r="AE4" s="1">
         <v>-2</v>
       </c>
       <c r="AF4" s="1">
         <v>0</v>
       </c>
-      <c r="AG4" s="1"/>
+      <c r="AG4" s="1">
+        <v>3</v>
+      </c>
       <c r="AH4" s="1">
         <v>-2</v>
       </c>
       <c r="AI4" s="1">
         <v>0</v>
       </c>
-      <c r="AJ4" s="1"/>
+      <c r="AJ4" s="1">
+        <v>1</v>
+      </c>
       <c r="AK4" s="1">
         <v>-2</v>
       </c>
       <c r="AL4" s="1">
         <v>0</v>
       </c>
-      <c r="AM4" s="1"/>
+      <c r="AM4" s="1">
+        <v>2</v>
+      </c>
       <c r="AN4" s="1">
         <v>-2</v>
       </c>
       <c r="AO4" s="1">
         <v>0</v>
       </c>
-      <c r="AP4" s="1"/>
+      <c r="AP4" s="1">
+        <v>3</v>
+      </c>
       <c r="AQ4" s="1">
         <v>-2</v>
       </c>
@@ -1089,56 +1230,72 @@
       <c r="AU4" s="1">
         <v>0</v>
       </c>
-      <c r="AV4" s="1"/>
+      <c r="AV4" s="1">
+        <v>2</v>
+      </c>
       <c r="AW4" s="1">
         <v>-2</v>
       </c>
       <c r="AX4" s="1">
         <v>0</v>
       </c>
-      <c r="AY4" s="1"/>
+      <c r="AY4" s="1">
+        <v>2</v>
+      </c>
       <c r="AZ4" s="1">
         <v>-2</v>
       </c>
       <c r="BA4" s="1">
         <v>0</v>
       </c>
-      <c r="BB4" s="1"/>
+      <c r="BB4" s="1">
+        <v>1</v>
+      </c>
       <c r="BC4" s="1">
         <v>-2</v>
       </c>
       <c r="BD4" s="1">
         <v>0</v>
       </c>
-      <c r="BE4" s="1"/>
+      <c r="BE4" s="1">
+        <v>4</v>
+      </c>
       <c r="BF4" s="1">
         <v>-2</v>
       </c>
       <c r="BG4" s="1">
         <v>0</v>
       </c>
-      <c r="BH4" s="1"/>
+      <c r="BH4" s="1">
+        <v>1</v>
+      </c>
       <c r="BI4" s="1">
         <v>-2</v>
       </c>
       <c r="BJ4" s="1">
         <v>0</v>
       </c>
-      <c r="BK4" s="1"/>
+      <c r="BK4" s="1">
+        <v>1</v>
+      </c>
       <c r="BL4" s="1">
         <v>-2</v>
       </c>
       <c r="BM4" s="1">
         <v>0</v>
       </c>
-      <c r="BN4" s="1"/>
+      <c r="BN4" s="1">
+        <v>1</v>
+      </c>
       <c r="BO4" s="1">
         <v>-2</v>
       </c>
       <c r="BP4" s="1">
         <v>0</v>
       </c>
-      <c r="BQ4" s="1"/>
+      <c r="BQ4" s="1">
+        <v>1</v>
+      </c>
       <c r="BR4" s="1"/>
       <c r="BS4" s="1"/>
       <c r="BT4" s="1"/>
@@ -4045,7 +4202,7 @@
       <c r="AY20" s="1"/>
       <c r="AZ20" s="1"/>
       <c r="BA20" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="BB20" s="1"/>
       <c r="BC20" s="1">
@@ -4333,7 +4490,7 @@
       <c r="AS22" s="1"/>
       <c r="AT22" s="1"/>
       <c r="AU22" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AV22" s="1"/>
       <c r="AW22" s="1"/>
@@ -4784,6 +4941,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
infos_filtres et eau pure
</commit_message>
<xml_diff>
--- a/datas_lab_IN.xlsx
+++ b/datas_lab_IN.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="17">
   <si>
     <t>About the codes</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t/>
+  </si>
+  <si>
+    <t>code</t>
   </si>
 </sst>
 </file>
@@ -446,10 +449,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CU32"/>
+  <dimension ref="A1:EX32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BS1" workbookViewId="0">
-      <selection activeCell="CC5" sqref="CC5"/>
+    <sheetView tabSelected="1" topLeftCell="DK1" workbookViewId="0">
+      <selection activeCell="DP4" sqref="DP4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -457,7 +460,7 @@
     <col min="3" max="3" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:99" ht="15.75" customHeight="1">
+    <row r="1" spans="1:154" ht="15.75" customHeight="1">
       <c r="A1" s="1">
         <v>217</v>
       </c>
@@ -642,26 +645,133 @@
         <v>42170</v>
       </c>
       <c r="CC1" s="2"/>
-      <c r="CD1" s="2"/>
-      <c r="CE1" s="2"/>
+      <c r="CD1" s="1">
+        <v>557</v>
+      </c>
+      <c r="CE1" s="2">
+        <v>42170</v>
+      </c>
       <c r="CF1" s="2"/>
-      <c r="CG1" s="2"/>
-      <c r="CH1" s="2"/>
+      <c r="CG1" s="1">
+        <v>560</v>
+      </c>
+      <c r="CH1" s="2">
+        <v>42170</v>
+      </c>
       <c r="CI1" s="2"/>
-      <c r="CJ1" s="2"/>
-      <c r="CK1" s="2"/>
+      <c r="CJ1" s="1">
+        <v>564</v>
+      </c>
+      <c r="CK1" s="2">
+        <v>42171</v>
+      </c>
       <c r="CL1" s="2"/>
-      <c r="CM1" s="2"/>
-      <c r="CN1" s="2"/>
+      <c r="CM1" s="1">
+        <v>567</v>
+      </c>
+      <c r="CN1" s="2">
+        <v>42171</v>
+      </c>
       <c r="CO1" s="2"/>
-      <c r="CP1" s="2"/>
-      <c r="CQ1" s="2"/>
+      <c r="CP1" s="1">
+        <v>570</v>
+      </c>
+      <c r="CQ1" s="2">
+        <v>42171</v>
+      </c>
       <c r="CR1" s="2"/>
-      <c r="CS1" s="2"/>
-      <c r="CT1" s="2"/>
+      <c r="CS1" s="1">
+        <v>575</v>
+      </c>
+      <c r="CT1" s="2">
+        <v>42171</v>
+      </c>
       <c r="CU1" s="2"/>
+      <c r="CV1" s="1">
+        <v>590</v>
+      </c>
+      <c r="CW1" s="2">
+        <v>42172</v>
+      </c>
+      <c r="CX1" s="2"/>
+      <c r="CY1" s="1">
+        <v>603</v>
+      </c>
+      <c r="CZ1" s="2">
+        <v>42172</v>
+      </c>
+      <c r="DA1" s="2"/>
+      <c r="DB1" s="1">
+        <v>605</v>
+      </c>
+      <c r="DC1" s="2">
+        <v>42172</v>
+      </c>
+      <c r="DD1" s="2"/>
+      <c r="DE1" s="1">
+        <v>642</v>
+      </c>
+      <c r="DF1" s="2">
+        <v>42172</v>
+      </c>
+      <c r="DG1" s="2"/>
+      <c r="DH1" s="1">
+        <v>644</v>
+      </c>
+      <c r="DI1" s="2">
+        <v>42172</v>
+      </c>
+      <c r="DJ1" s="2"/>
+      <c r="DK1" s="1">
+        <v>565</v>
+      </c>
+      <c r="DL1" s="2">
+        <v>42173</v>
+      </c>
+      <c r="DM1" s="2"/>
+      <c r="DN1" s="1">
+        <v>566</v>
+      </c>
+      <c r="DO1" s="2">
+        <v>42173</v>
+      </c>
+      <c r="DP1" s="2"/>
+      <c r="DQ1" s="2"/>
+      <c r="DR1" s="2"/>
+      <c r="DS1" s="2"/>
+      <c r="DT1" s="2"/>
+      <c r="DU1" s="2"/>
+      <c r="DV1" s="2"/>
+      <c r="DW1" s="2"/>
+      <c r="DX1" s="2"/>
+      <c r="DY1" s="2"/>
+      <c r="DZ1" s="2"/>
+      <c r="EA1" s="2"/>
+      <c r="EB1" s="2"/>
+      <c r="EC1" s="2"/>
+      <c r="ED1" s="2"/>
+      <c r="EE1" s="2"/>
+      <c r="EF1" s="2"/>
+      <c r="EG1" s="2"/>
+      <c r="EH1" s="2"/>
+      <c r="EI1" s="2"/>
+      <c r="EJ1" s="2"/>
+      <c r="EK1" s="2"/>
+      <c r="EL1" s="2"/>
+      <c r="EM1" s="2"/>
+      <c r="EN1" s="2"/>
+      <c r="EO1" s="2"/>
+      <c r="EP1" s="2"/>
+      <c r="EQ1" s="2"/>
+      <c r="ER1" s="2"/>
+      <c r="ES1" s="2"/>
+      <c r="ET1" s="2"/>
+      <c r="EU1" s="2"/>
+      <c r="EV1" s="2"/>
+      <c r="EW1" s="2"/>
+      <c r="EX1" s="2"/>
     </row>
-    <row r="2" spans="1:99" ht="15.75" customHeight="1">
+    <row r="2" spans="1:154" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -843,29 +953,136 @@
       <c r="CB2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="CC2" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD2" s="1"/>
-      <c r="CE2" s="1"/>
+      <c r="CC2" s="1"/>
+      <c r="CD2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CE2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CF2" s="1"/>
-      <c r="CG2" s="1"/>
-      <c r="CH2" s="1"/>
+      <c r="CG2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CH2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CI2" s="1"/>
-      <c r="CJ2" s="1"/>
-      <c r="CK2" s="1"/>
+      <c r="CJ2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CK2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CL2" s="1"/>
-      <c r="CM2" s="1"/>
-      <c r="CN2" s="1"/>
+      <c r="CM2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CN2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CO2" s="1"/>
-      <c r="CP2" s="1"/>
-      <c r="CQ2" s="1"/>
+      <c r="CP2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CQ2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CR2" s="1"/>
-      <c r="CS2" s="1"/>
-      <c r="CT2" s="1"/>
+      <c r="CS2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CT2" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="CU2" s="1"/>
+      <c r="CV2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CW2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="CX2" s="1"/>
+      <c r="CY2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="CZ2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DA2" s="1"/>
+      <c r="DB2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DC2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DD2" s="1"/>
+      <c r="DE2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DF2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DG2" s="1"/>
+      <c r="DH2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DI2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DJ2" s="1"/>
+      <c r="DK2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DL2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DM2" s="1"/>
+      <c r="DN2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="DO2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="DP2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="DQ2" s="1"/>
+      <c r="DR2" s="1"/>
+      <c r="DS2" s="1"/>
+      <c r="DT2" s="1"/>
+      <c r="DU2" s="1"/>
+      <c r="DV2" s="1"/>
+      <c r="DW2" s="1"/>
+      <c r="DX2" s="1"/>
+      <c r="DY2" s="1"/>
+      <c r="DZ2" s="1"/>
+      <c r="EA2" s="1"/>
+      <c r="EB2" s="1"/>
+      <c r="EC2" s="1"/>
+      <c r="ED2" s="1"/>
+      <c r="EE2" s="1"/>
+      <c r="EF2" s="1"/>
+      <c r="EG2" s="1"/>
+      <c r="EH2" s="1"/>
+      <c r="EI2" s="1"/>
+      <c r="EJ2" s="1"/>
+      <c r="EK2" s="1"/>
+      <c r="EL2" s="1"/>
+      <c r="EM2" s="1"/>
+      <c r="EN2" s="1"/>
+      <c r="EO2" s="1"/>
+      <c r="EP2" s="1"/>
+      <c r="EQ2" s="1"/>
+      <c r="ER2" s="1"/>
+      <c r="ES2" s="1"/>
+      <c r="ET2" s="1"/>
+      <c r="EU2" s="1"/>
+      <c r="EV2" s="1"/>
+      <c r="EW2" s="1"/>
+      <c r="EX2" s="1"/>
     </row>
-    <row r="3" spans="1:99" ht="15.75" customHeight="1">
+    <row r="3" spans="1:154" ht="15.75" customHeight="1">
       <c r="A3" s="1">
         <v>-1</v>
       </c>
@@ -1047,26 +1264,135 @@
         <v>0</v>
       </c>
       <c r="CC3" s="1"/>
-      <c r="CD3" s="1"/>
-      <c r="CE3" s="1"/>
+      <c r="CD3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CE3" s="1">
+        <v>0</v>
+      </c>
       <c r="CF3" s="1"/>
-      <c r="CG3" s="1"/>
-      <c r="CH3" s="1"/>
+      <c r="CG3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CH3" s="1">
+        <v>0</v>
+      </c>
       <c r="CI3" s="1"/>
-      <c r="CJ3" s="1"/>
-      <c r="CK3" s="1"/>
+      <c r="CJ3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CK3" s="1">
+        <v>0</v>
+      </c>
       <c r="CL3" s="1"/>
-      <c r="CM3" s="1"/>
-      <c r="CN3" s="1"/>
+      <c r="CM3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CN3" s="1">
+        <v>0</v>
+      </c>
       <c r="CO3" s="1"/>
-      <c r="CP3" s="1"/>
-      <c r="CQ3" s="1"/>
+      <c r="CP3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CQ3" s="1">
+        <v>0</v>
+      </c>
       <c r="CR3" s="1"/>
-      <c r="CS3" s="1"/>
-      <c r="CT3" s="1"/>
+      <c r="CS3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CT3" s="1">
+        <v>0</v>
+      </c>
       <c r="CU3" s="1"/>
+      <c r="CV3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CW3" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX3" s="1"/>
+      <c r="CY3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="CZ3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA3" s="1"/>
+      <c r="DB3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="DC3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD3" s="1"/>
+      <c r="DE3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="DF3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG3" s="1"/>
+      <c r="DH3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="DI3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ3" s="1"/>
+      <c r="DK3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="DL3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM3" s="1"/>
+      <c r="DN3" s="1">
+        <v>-1</v>
+      </c>
+      <c r="DO3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP3" s="1">
+        <v>0</v>
+      </c>
+      <c r="DQ3" s="1"/>
+      <c r="DR3" s="1"/>
+      <c r="DS3" s="1"/>
+      <c r="DT3" s="1"/>
+      <c r="DU3" s="1"/>
+      <c r="DV3" s="1"/>
+      <c r="DW3" s="1"/>
+      <c r="DX3" s="1"/>
+      <c r="DY3" s="1"/>
+      <c r="DZ3" s="1"/>
+      <c r="EA3" s="1"/>
+      <c r="EB3" s="1"/>
+      <c r="EC3" s="1"/>
+      <c r="ED3" s="1"/>
+      <c r="EE3" s="1"/>
+      <c r="EF3" s="1"/>
+      <c r="EG3" s="1"/>
+      <c r="EH3" s="1"/>
+      <c r="EI3" s="1"/>
+      <c r="EJ3" s="1"/>
+      <c r="EK3" s="1"/>
+      <c r="EL3" s="1"/>
+      <c r="EM3" s="1"/>
+      <c r="EN3" s="1"/>
+      <c r="EO3" s="1"/>
+      <c r="EP3" s="1"/>
+      <c r="EQ3" s="1"/>
+      <c r="ER3" s="1"/>
+      <c r="ES3" s="1"/>
+      <c r="ET3" s="1"/>
+      <c r="EU3" s="1"/>
+      <c r="EV3" s="1"/>
+      <c r="EW3" s="1"/>
+      <c r="EX3" s="1"/>
     </row>
-    <row r="4" spans="1:99" ht="15.75" customHeight="1">
+    <row r="4" spans="1:154" ht="15.75" customHeight="1">
       <c r="A4" s="1">
         <v>-2</v>
       </c>
@@ -1248,26 +1574,133 @@
         <v>0</v>
       </c>
       <c r="CC4" s="1"/>
-      <c r="CD4" s="1"/>
-      <c r="CE4" s="1"/>
+      <c r="CD4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CE4" s="1">
+        <v>0</v>
+      </c>
       <c r="CF4" s="1"/>
-      <c r="CG4" s="1"/>
-      <c r="CH4" s="1"/>
+      <c r="CG4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CH4" s="1">
+        <v>0</v>
+      </c>
       <c r="CI4" s="1"/>
-      <c r="CJ4" s="1"/>
-      <c r="CK4" s="1"/>
+      <c r="CJ4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CK4" s="1">
+        <v>0</v>
+      </c>
       <c r="CL4" s="1"/>
-      <c r="CM4" s="1"/>
-      <c r="CN4" s="1"/>
+      <c r="CM4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CN4" s="1">
+        <v>0</v>
+      </c>
       <c r="CO4" s="1"/>
-      <c r="CP4" s="1"/>
-      <c r="CQ4" s="1"/>
+      <c r="CP4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CQ4" s="1">
+        <v>0</v>
+      </c>
       <c r="CR4" s="1"/>
-      <c r="CS4" s="1"/>
-      <c r="CT4" s="1"/>
+      <c r="CS4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CT4" s="1">
+        <v>0</v>
+      </c>
       <c r="CU4" s="1"/>
+      <c r="CV4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CW4" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX4" s="1"/>
+      <c r="CY4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="CZ4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA4" s="1"/>
+      <c r="DB4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="DC4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD4" s="1"/>
+      <c r="DE4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="DF4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG4" s="1"/>
+      <c r="DH4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="DI4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ4" s="1"/>
+      <c r="DK4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="DL4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM4" s="1"/>
+      <c r="DN4" s="1">
+        <v>-2</v>
+      </c>
+      <c r="DO4" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP4" s="1"/>
+      <c r="DQ4" s="1"/>
+      <c r="DR4" s="1"/>
+      <c r="DS4" s="1"/>
+      <c r="DT4" s="1"/>
+      <c r="DU4" s="1"/>
+      <c r="DV4" s="1"/>
+      <c r="DW4" s="1"/>
+      <c r="DX4" s="1"/>
+      <c r="DY4" s="1"/>
+      <c r="DZ4" s="1"/>
+      <c r="EA4" s="1"/>
+      <c r="EB4" s="1"/>
+      <c r="EC4" s="1"/>
+      <c r="ED4" s="1"/>
+      <c r="EE4" s="1"/>
+      <c r="EF4" s="1"/>
+      <c r="EG4" s="1"/>
+      <c r="EH4" s="1"/>
+      <c r="EI4" s="1"/>
+      <c r="EJ4" s="1"/>
+      <c r="EK4" s="1"/>
+      <c r="EL4" s="1"/>
+      <c r="EM4" s="1"/>
+      <c r="EN4" s="1"/>
+      <c r="EO4" s="1"/>
+      <c r="EP4" s="1"/>
+      <c r="EQ4" s="1"/>
+      <c r="ER4" s="1"/>
+      <c r="ES4" s="1"/>
+      <c r="ET4" s="1"/>
+      <c r="EU4" s="1"/>
+      <c r="EV4" s="1"/>
+      <c r="EW4" s="1"/>
+      <c r="EX4" s="1"/>
     </row>
-    <row r="5" spans="1:99" ht="15.75" customHeight="1">
+    <row r="5" spans="1:154" ht="15.75" customHeight="1">
       <c r="A5" s="1">
         <v>-3</v>
       </c>
@@ -1449,26 +1882,133 @@
         <v>0</v>
       </c>
       <c r="CC5" s="1"/>
-      <c r="CD5" s="1"/>
-      <c r="CE5" s="1"/>
+      <c r="CD5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CE5" s="1">
+        <v>0</v>
+      </c>
       <c r="CF5" s="1"/>
-      <c r="CG5" s="1"/>
-      <c r="CH5" s="1"/>
+      <c r="CG5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CH5" s="1">
+        <v>0</v>
+      </c>
       <c r="CI5" s="1"/>
-      <c r="CJ5" s="1"/>
-      <c r="CK5" s="1"/>
+      <c r="CJ5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CK5" s="1">
+        <v>0</v>
+      </c>
       <c r="CL5" s="1"/>
-      <c r="CM5" s="1"/>
-      <c r="CN5" s="1"/>
+      <c r="CM5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CN5" s="1">
+        <v>0</v>
+      </c>
       <c r="CO5" s="1"/>
-      <c r="CP5" s="1"/>
-      <c r="CQ5" s="1"/>
+      <c r="CP5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CQ5" s="1">
+        <v>0</v>
+      </c>
       <c r="CR5" s="1"/>
-      <c r="CS5" s="1"/>
-      <c r="CT5" s="1"/>
+      <c r="CS5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CT5" s="1">
+        <v>0</v>
+      </c>
       <c r="CU5" s="1"/>
+      <c r="CV5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CW5" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX5" s="1"/>
+      <c r="CY5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="CZ5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA5" s="1"/>
+      <c r="DB5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="DC5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD5" s="1"/>
+      <c r="DE5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="DF5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG5" s="1"/>
+      <c r="DH5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="DI5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ5" s="1"/>
+      <c r="DK5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="DL5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM5" s="1"/>
+      <c r="DN5" s="1">
+        <v>-3</v>
+      </c>
+      <c r="DO5" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP5" s="1"/>
+      <c r="DQ5" s="1"/>
+      <c r="DR5" s="1"/>
+      <c r="DS5" s="1"/>
+      <c r="DT5" s="1"/>
+      <c r="DU5" s="1"/>
+      <c r="DV5" s="1"/>
+      <c r="DW5" s="1"/>
+      <c r="DX5" s="1"/>
+      <c r="DY5" s="1"/>
+      <c r="DZ5" s="1"/>
+      <c r="EA5" s="1"/>
+      <c r="EB5" s="1"/>
+      <c r="EC5" s="1"/>
+      <c r="ED5" s="1"/>
+      <c r="EE5" s="1"/>
+      <c r="EF5" s="1"/>
+      <c r="EG5" s="1"/>
+      <c r="EH5" s="1"/>
+      <c r="EI5" s="1"/>
+      <c r="EJ5" s="1"/>
+      <c r="EK5" s="1"/>
+      <c r="EL5" s="1"/>
+      <c r="EM5" s="1"/>
+      <c r="EN5" s="1"/>
+      <c r="EO5" s="1"/>
+      <c r="EP5" s="1"/>
+      <c r="EQ5" s="1"/>
+      <c r="ER5" s="1"/>
+      <c r="ES5" s="1"/>
+      <c r="ET5" s="1"/>
+      <c r="EU5" s="1"/>
+      <c r="EV5" s="1"/>
+      <c r="EW5" s="1"/>
+      <c r="EX5" s="1"/>
     </row>
-    <row r="6" spans="1:99" ht="15.75" customHeight="1">
+    <row r="6" spans="1:154" ht="15.75" customHeight="1">
       <c r="A6" s="1">
         <v>-4</v>
       </c>
@@ -1650,26 +2190,133 @@
         <v>0</v>
       </c>
       <c r="CC6" s="1"/>
-      <c r="CD6" s="1"/>
-      <c r="CE6" s="1"/>
+      <c r="CD6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CE6" s="1">
+        <v>0</v>
+      </c>
       <c r="CF6" s="1"/>
-      <c r="CG6" s="1"/>
-      <c r="CH6" s="1"/>
+      <c r="CG6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CH6" s="1">
+        <v>0</v>
+      </c>
       <c r="CI6" s="1"/>
-      <c r="CJ6" s="1"/>
-      <c r="CK6" s="1"/>
+      <c r="CJ6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CK6" s="1">
+        <v>0</v>
+      </c>
       <c r="CL6" s="1"/>
-      <c r="CM6" s="1"/>
-      <c r="CN6" s="1"/>
+      <c r="CM6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CN6" s="1">
+        <v>0</v>
+      </c>
       <c r="CO6" s="1"/>
-      <c r="CP6" s="1"/>
-      <c r="CQ6" s="1"/>
+      <c r="CP6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CQ6" s="1">
+        <v>0</v>
+      </c>
       <c r="CR6" s="1"/>
-      <c r="CS6" s="1"/>
-      <c r="CT6" s="1"/>
+      <c r="CS6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CT6" s="1">
+        <v>0</v>
+      </c>
       <c r="CU6" s="1"/>
+      <c r="CV6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CW6" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX6" s="1"/>
+      <c r="CY6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="CZ6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA6" s="1"/>
+      <c r="DB6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="DC6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD6" s="1"/>
+      <c r="DE6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="DF6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG6" s="1"/>
+      <c r="DH6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="DI6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ6" s="1"/>
+      <c r="DK6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="DL6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM6" s="1"/>
+      <c r="DN6" s="1">
+        <v>-4</v>
+      </c>
+      <c r="DO6" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP6" s="1"/>
+      <c r="DQ6" s="1"/>
+      <c r="DR6" s="1"/>
+      <c r="DS6" s="1"/>
+      <c r="DT6" s="1"/>
+      <c r="DU6" s="1"/>
+      <c r="DV6" s="1"/>
+      <c r="DW6" s="1"/>
+      <c r="DX6" s="1"/>
+      <c r="DY6" s="1"/>
+      <c r="DZ6" s="1"/>
+      <c r="EA6" s="1"/>
+      <c r="EB6" s="1"/>
+      <c r="EC6" s="1"/>
+      <c r="ED6" s="1"/>
+      <c r="EE6" s="1"/>
+      <c r="EF6" s="1"/>
+      <c r="EG6" s="1"/>
+      <c r="EH6" s="1"/>
+      <c r="EI6" s="1"/>
+      <c r="EJ6" s="1"/>
+      <c r="EK6" s="1"/>
+      <c r="EL6" s="1"/>
+      <c r="EM6" s="1"/>
+      <c r="EN6" s="1"/>
+      <c r="EO6" s="1"/>
+      <c r="EP6" s="1"/>
+      <c r="EQ6" s="1"/>
+      <c r="ER6" s="1"/>
+      <c r="ES6" s="1"/>
+      <c r="ET6" s="1"/>
+      <c r="EU6" s="1"/>
+      <c r="EV6" s="1"/>
+      <c r="EW6" s="1"/>
+      <c r="EX6" s="1"/>
     </row>
-    <row r="7" spans="1:99" ht="15.75" customHeight="1">
+    <row r="7" spans="1:154" ht="15.75" customHeight="1">
       <c r="A7" s="1">
         <v>-5</v>
       </c>
@@ -1851,26 +2498,133 @@
         <v>0</v>
       </c>
       <c r="CC7" s="1"/>
-      <c r="CD7" s="1"/>
-      <c r="CE7" s="1"/>
+      <c r="CD7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CE7" s="1">
+        <v>0</v>
+      </c>
       <c r="CF7" s="1"/>
-      <c r="CG7" s="1"/>
-      <c r="CH7" s="1"/>
+      <c r="CG7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CH7" s="1">
+        <v>0</v>
+      </c>
       <c r="CI7" s="1"/>
-      <c r="CJ7" s="1"/>
-      <c r="CK7" s="1"/>
+      <c r="CJ7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CK7" s="1">
+        <v>0</v>
+      </c>
       <c r="CL7" s="1"/>
-      <c r="CM7" s="1"/>
-      <c r="CN7" s="1"/>
+      <c r="CM7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CN7" s="1">
+        <v>0</v>
+      </c>
       <c r="CO7" s="1"/>
-      <c r="CP7" s="1"/>
-      <c r="CQ7" s="1"/>
+      <c r="CP7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CQ7" s="1">
+        <v>0</v>
+      </c>
       <c r="CR7" s="1"/>
-      <c r="CS7" s="1"/>
-      <c r="CT7" s="1"/>
+      <c r="CS7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CT7" s="1">
+        <v>0</v>
+      </c>
       <c r="CU7" s="1"/>
+      <c r="CV7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CW7" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX7" s="1"/>
+      <c r="CY7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="CZ7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA7" s="1"/>
+      <c r="DB7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="DC7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD7" s="1"/>
+      <c r="DE7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="DF7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG7" s="1"/>
+      <c r="DH7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="DI7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ7" s="1"/>
+      <c r="DK7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="DL7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DM7" s="1"/>
+      <c r="DN7" s="1">
+        <v>-5</v>
+      </c>
+      <c r="DO7" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP7" s="1"/>
+      <c r="DQ7" s="1"/>
+      <c r="DR7" s="1"/>
+      <c r="DS7" s="1"/>
+      <c r="DT7" s="1"/>
+      <c r="DU7" s="1"/>
+      <c r="DV7" s="1"/>
+      <c r="DW7" s="1"/>
+      <c r="DX7" s="1"/>
+      <c r="DY7" s="1"/>
+      <c r="DZ7" s="1"/>
+      <c r="EA7" s="1"/>
+      <c r="EB7" s="1"/>
+      <c r="EC7" s="1"/>
+      <c r="ED7" s="1"/>
+      <c r="EE7" s="1"/>
+      <c r="EF7" s="1"/>
+      <c r="EG7" s="1"/>
+      <c r="EH7" s="1"/>
+      <c r="EI7" s="1"/>
+      <c r="EJ7" s="1"/>
+      <c r="EK7" s="1"/>
+      <c r="EL7" s="1"/>
+      <c r="EM7" s="1"/>
+      <c r="EN7" s="1"/>
+      <c r="EO7" s="1"/>
+      <c r="EP7" s="1"/>
+      <c r="EQ7" s="1"/>
+      <c r="ER7" s="1"/>
+      <c r="ES7" s="1"/>
+      <c r="ET7" s="1"/>
+      <c r="EU7" s="1"/>
+      <c r="EV7" s="1"/>
+      <c r="EW7" s="1"/>
+      <c r="EX7" s="1"/>
     </row>
-    <row r="8" spans="1:99" ht="15.75" customHeight="1">
+    <row r="8" spans="1:154" ht="15.75" customHeight="1">
       <c r="A8" s="1">
         <v>-6</v>
       </c>
@@ -2052,26 +2806,133 @@
         <v>0</v>
       </c>
       <c r="CC8" s="1"/>
-      <c r="CD8" s="1"/>
-      <c r="CE8" s="1"/>
+      <c r="CD8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CE8" s="1">
+        <v>0</v>
+      </c>
       <c r="CF8" s="1"/>
-      <c r="CG8" s="1"/>
-      <c r="CH8" s="1"/>
+      <c r="CG8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CH8" s="1">
+        <v>0</v>
+      </c>
       <c r="CI8" s="1"/>
-      <c r="CJ8" s="1"/>
-      <c r="CK8" s="1"/>
+      <c r="CJ8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CK8" s="1">
+        <v>0</v>
+      </c>
       <c r="CL8" s="1"/>
-      <c r="CM8" s="1"/>
-      <c r="CN8" s="1"/>
+      <c r="CM8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CN8" s="1">
+        <v>1</v>
+      </c>
       <c r="CO8" s="1"/>
-      <c r="CP8" s="1"/>
-      <c r="CQ8" s="1"/>
+      <c r="CP8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CQ8" s="1">
+        <v>0</v>
+      </c>
       <c r="CR8" s="1"/>
-      <c r="CS8" s="1"/>
-      <c r="CT8" s="1"/>
+      <c r="CS8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CT8" s="1">
+        <v>0</v>
+      </c>
       <c r="CU8" s="1"/>
+      <c r="CV8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CW8" s="1">
+        <v>0</v>
+      </c>
+      <c r="CX8" s="1"/>
+      <c r="CY8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="CZ8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA8" s="1"/>
+      <c r="DB8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="DC8" s="1">
+        <v>2</v>
+      </c>
+      <c r="DD8" s="1"/>
+      <c r="DE8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="DF8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DG8" s="1"/>
+      <c r="DH8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="DI8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ8" s="1"/>
+      <c r="DK8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="DL8" s="1">
+        <v>6</v>
+      </c>
+      <c r="DM8" s="1"/>
+      <c r="DN8" s="1">
+        <v>-6</v>
+      </c>
+      <c r="DO8" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP8" s="1"/>
+      <c r="DQ8" s="1"/>
+      <c r="DR8" s="1"/>
+      <c r="DS8" s="1"/>
+      <c r="DT8" s="1"/>
+      <c r="DU8" s="1"/>
+      <c r="DV8" s="1"/>
+      <c r="DW8" s="1"/>
+      <c r="DX8" s="1"/>
+      <c r="DY8" s="1"/>
+      <c r="DZ8" s="1"/>
+      <c r="EA8" s="1"/>
+      <c r="EB8" s="1"/>
+      <c r="EC8" s="1"/>
+      <c r="ED8" s="1"/>
+      <c r="EE8" s="1"/>
+      <c r="EF8" s="1"/>
+      <c r="EG8" s="1"/>
+      <c r="EH8" s="1"/>
+      <c r="EI8" s="1"/>
+      <c r="EJ8" s="1"/>
+      <c r="EK8" s="1"/>
+      <c r="EL8" s="1"/>
+      <c r="EM8" s="1"/>
+      <c r="EN8" s="1"/>
+      <c r="EO8" s="1"/>
+      <c r="EP8" s="1"/>
+      <c r="EQ8" s="1"/>
+      <c r="ER8" s="1"/>
+      <c r="ES8" s="1"/>
+      <c r="ET8" s="1"/>
+      <c r="EU8" s="1"/>
+      <c r="EV8" s="1"/>
+      <c r="EW8" s="1"/>
+      <c r="EX8" s="1"/>
     </row>
-    <row r="9" spans="1:99" ht="15.75" customHeight="1">
+    <row r="9" spans="1:154" ht="15.75" customHeight="1">
       <c r="A9" s="1">
         <v>-7</v>
       </c>
@@ -2253,26 +3114,133 @@
         <v>0</v>
       </c>
       <c r="CC9" s="1"/>
-      <c r="CD9" s="1"/>
-      <c r="CE9" s="1"/>
+      <c r="CD9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CE9" s="1">
+        <v>2</v>
+      </c>
       <c r="CF9" s="1"/>
-      <c r="CG9" s="1"/>
-      <c r="CH9" s="1"/>
+      <c r="CG9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CH9" s="1">
+        <v>0</v>
+      </c>
       <c r="CI9" s="1"/>
-      <c r="CJ9" s="1"/>
-      <c r="CK9" s="1"/>
+      <c r="CJ9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CK9" s="1">
+        <v>0</v>
+      </c>
       <c r="CL9" s="1"/>
-      <c r="CM9" s="1"/>
-      <c r="CN9" s="1"/>
+      <c r="CM9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CN9" s="1">
+        <v>1</v>
+      </c>
       <c r="CO9" s="1"/>
-      <c r="CP9" s="1"/>
-      <c r="CQ9" s="1"/>
+      <c r="CP9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CQ9" s="1">
+        <v>0</v>
+      </c>
       <c r="CR9" s="1"/>
-      <c r="CS9" s="1"/>
-      <c r="CT9" s="1"/>
+      <c r="CS9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CT9" s="1">
+        <v>0</v>
+      </c>
       <c r="CU9" s="1"/>
+      <c r="CV9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CW9" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX9" s="1"/>
+      <c r="CY9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="CZ9" s="1">
+        <v>1</v>
+      </c>
+      <c r="DA9" s="1"/>
+      <c r="DB9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="DC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD9" s="1"/>
+      <c r="DE9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="DF9" s="1">
+        <v>4</v>
+      </c>
+      <c r="DG9" s="1"/>
+      <c r="DH9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="DI9" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ9" s="1"/>
+      <c r="DK9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="DL9" s="1">
+        <v>9</v>
+      </c>
+      <c r="DM9" s="1"/>
+      <c r="DN9" s="1">
+        <v>-7</v>
+      </c>
+      <c r="DO9" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP9" s="1"/>
+      <c r="DQ9" s="1"/>
+      <c r="DR9" s="1"/>
+      <c r="DS9" s="1"/>
+      <c r="DT9" s="1"/>
+      <c r="DU9" s="1"/>
+      <c r="DV9" s="1"/>
+      <c r="DW9" s="1"/>
+      <c r="DX9" s="1"/>
+      <c r="DY9" s="1"/>
+      <c r="DZ9" s="1"/>
+      <c r="EA9" s="1"/>
+      <c r="EB9" s="1"/>
+      <c r="EC9" s="1"/>
+      <c r="ED9" s="1"/>
+      <c r="EE9" s="1"/>
+      <c r="EF9" s="1"/>
+      <c r="EG9" s="1"/>
+      <c r="EH9" s="1"/>
+      <c r="EI9" s="1"/>
+      <c r="EJ9" s="1"/>
+      <c r="EK9" s="1"/>
+      <c r="EL9" s="1"/>
+      <c r="EM9" s="1"/>
+      <c r="EN9" s="1"/>
+      <c r="EO9" s="1"/>
+      <c r="EP9" s="1"/>
+      <c r="EQ9" s="1"/>
+      <c r="ER9" s="1"/>
+      <c r="ES9" s="1"/>
+      <c r="ET9" s="1"/>
+      <c r="EU9" s="1"/>
+      <c r="EV9" s="1"/>
+      <c r="EW9" s="1"/>
+      <c r="EX9" s="1"/>
     </row>
-    <row r="10" spans="1:99" ht="15.75" customHeight="1">
+    <row r="10" spans="1:154" ht="15.75" customHeight="1">
       <c r="A10" s="1">
         <v>-8</v>
       </c>
@@ -2454,26 +3422,133 @@
         <v>0</v>
       </c>
       <c r="CC10" s="1"/>
-      <c r="CD10" s="1"/>
-      <c r="CE10" s="1"/>
+      <c r="CD10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CE10" s="1">
+        <v>1</v>
+      </c>
       <c r="CF10" s="1"/>
-      <c r="CG10" s="1"/>
-      <c r="CH10" s="1"/>
+      <c r="CG10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CH10" s="1">
+        <v>0</v>
+      </c>
       <c r="CI10" s="1"/>
-      <c r="CJ10" s="1"/>
-      <c r="CK10" s="1"/>
+      <c r="CJ10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CK10" s="1">
+        <v>2</v>
+      </c>
       <c r="CL10" s="1"/>
-      <c r="CM10" s="1"/>
-      <c r="CN10" s="1"/>
+      <c r="CM10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CN10" s="1">
+        <v>1</v>
+      </c>
       <c r="CO10" s="1"/>
-      <c r="CP10" s="1"/>
-      <c r="CQ10" s="1"/>
+      <c r="CP10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CQ10" s="1">
+        <v>3</v>
+      </c>
       <c r="CR10" s="1"/>
-      <c r="CS10" s="1"/>
-      <c r="CT10" s="1"/>
+      <c r="CS10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CT10" s="1">
+        <v>0</v>
+      </c>
       <c r="CU10" s="1"/>
+      <c r="CV10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CW10" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX10" s="1"/>
+      <c r="CY10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="CZ10" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA10" s="1"/>
+      <c r="DB10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="DC10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD10" s="1"/>
+      <c r="DE10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="DF10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DG10" s="1"/>
+      <c r="DH10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="DI10" s="1">
+        <v>0</v>
+      </c>
+      <c r="DJ10" s="1"/>
+      <c r="DK10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="DL10" s="1">
+        <v>4</v>
+      </c>
+      <c r="DM10" s="1"/>
+      <c r="DN10" s="1">
+        <v>-8</v>
+      </c>
+      <c r="DO10" s="1">
+        <v>1</v>
+      </c>
+      <c r="DP10" s="1"/>
+      <c r="DQ10" s="1"/>
+      <c r="DR10" s="1"/>
+      <c r="DS10" s="1"/>
+      <c r="DT10" s="1"/>
+      <c r="DU10" s="1"/>
+      <c r="DV10" s="1"/>
+      <c r="DW10" s="1"/>
+      <c r="DX10" s="1"/>
+      <c r="DY10" s="1"/>
+      <c r="DZ10" s="1"/>
+      <c r="EA10" s="1"/>
+      <c r="EB10" s="1"/>
+      <c r="EC10" s="1"/>
+      <c r="ED10" s="1"/>
+      <c r="EE10" s="1"/>
+      <c r="EF10" s="1"/>
+      <c r="EG10" s="1"/>
+      <c r="EH10" s="1"/>
+      <c r="EI10" s="1"/>
+      <c r="EJ10" s="1"/>
+      <c r="EK10" s="1"/>
+      <c r="EL10" s="1"/>
+      <c r="EM10" s="1"/>
+      <c r="EN10" s="1"/>
+      <c r="EO10" s="1"/>
+      <c r="EP10" s="1"/>
+      <c r="EQ10" s="1"/>
+      <c r="ER10" s="1"/>
+      <c r="ES10" s="1"/>
+      <c r="ET10" s="1"/>
+      <c r="EU10" s="1"/>
+      <c r="EV10" s="1"/>
+      <c r="EW10" s="1"/>
+      <c r="EX10" s="1"/>
     </row>
-    <row r="11" spans="1:99" ht="15.75" customHeight="1">
+    <row r="11" spans="1:154" ht="15.75" customHeight="1">
       <c r="A11" s="1">
         <v>-8.5</v>
       </c>
@@ -2655,26 +3730,133 @@
         <v>1</v>
       </c>
       <c r="CC11" s="1"/>
-      <c r="CD11" s="1"/>
-      <c r="CE11" s="1"/>
+      <c r="CD11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CE11" s="1">
+        <v>4</v>
+      </c>
       <c r="CF11" s="1"/>
-      <c r="CG11" s="1"/>
-      <c r="CH11" s="1"/>
+      <c r="CG11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CH11" s="1">
+        <v>3</v>
+      </c>
       <c r="CI11" s="1"/>
-      <c r="CJ11" s="1"/>
-      <c r="CK11" s="1"/>
+      <c r="CJ11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CK11" s="1">
+        <v>0</v>
+      </c>
       <c r="CL11" s="1"/>
-      <c r="CM11" s="1"/>
-      <c r="CN11" s="1"/>
+      <c r="CM11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CN11" s="1">
+        <v>2</v>
+      </c>
       <c r="CO11" s="1"/>
-      <c r="CP11" s="1"/>
-      <c r="CQ11" s="1"/>
+      <c r="CP11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CQ11" s="1">
+        <v>4</v>
+      </c>
       <c r="CR11" s="1"/>
-      <c r="CS11" s="1"/>
-      <c r="CT11" s="1"/>
+      <c r="CS11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CT11" s="1">
+        <v>1</v>
+      </c>
       <c r="CU11" s="1"/>
+      <c r="CV11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CW11" s="1">
+        <v>5</v>
+      </c>
+      <c r="CX11" s="1"/>
+      <c r="CY11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="CZ11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA11" s="1"/>
+      <c r="DB11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="DC11" s="1">
+        <v>12</v>
+      </c>
+      <c r="DD11" s="1"/>
+      <c r="DE11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="DF11" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG11" s="1"/>
+      <c r="DH11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="DI11" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ11" s="1"/>
+      <c r="DK11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="DL11" s="1">
+        <v>11</v>
+      </c>
+      <c r="DM11" s="1"/>
+      <c r="DN11" s="1">
+        <v>-9</v>
+      </c>
+      <c r="DO11" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP11" s="1"/>
+      <c r="DQ11" s="1"/>
+      <c r="DR11" s="1"/>
+      <c r="DS11" s="1"/>
+      <c r="DT11" s="1"/>
+      <c r="DU11" s="1"/>
+      <c r="DV11" s="1"/>
+      <c r="DW11" s="1"/>
+      <c r="DX11" s="1"/>
+      <c r="DY11" s="1"/>
+      <c r="DZ11" s="1"/>
+      <c r="EA11" s="1"/>
+      <c r="EB11" s="1"/>
+      <c r="EC11" s="1"/>
+      <c r="ED11" s="1"/>
+      <c r="EE11" s="1"/>
+      <c r="EF11" s="1"/>
+      <c r="EG11" s="1"/>
+      <c r="EH11" s="1"/>
+      <c r="EI11" s="1"/>
+      <c r="EJ11" s="1"/>
+      <c r="EK11" s="1"/>
+      <c r="EL11" s="1"/>
+      <c r="EM11" s="1"/>
+      <c r="EN11" s="1"/>
+      <c r="EO11" s="1"/>
+      <c r="EP11" s="1"/>
+      <c r="EQ11" s="1"/>
+      <c r="ER11" s="1"/>
+      <c r="ES11" s="1"/>
+      <c r="ET11" s="1"/>
+      <c r="EU11" s="1"/>
+      <c r="EV11" s="1"/>
+      <c r="EW11" s="1"/>
+      <c r="EX11" s="1"/>
     </row>
-    <row r="12" spans="1:99" ht="15.75" customHeight="1">
+    <row r="12" spans="1:154" ht="15.75" customHeight="1">
       <c r="A12" s="1">
         <v>-9</v>
       </c>
@@ -2851,26 +4033,133 @@
         <v>4</v>
       </c>
       <c r="CC12" s="1"/>
-      <c r="CD12" s="1"/>
-      <c r="CE12" s="1"/>
+      <c r="CD12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CE12" s="1">
+        <v>4</v>
+      </c>
       <c r="CF12" s="1"/>
-      <c r="CG12" s="1"/>
-      <c r="CH12" s="1"/>
+      <c r="CG12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CH12" s="1">
+        <v>1</v>
+      </c>
       <c r="CI12" s="1"/>
-      <c r="CJ12" s="1"/>
-      <c r="CK12" s="1"/>
+      <c r="CJ12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CK12" s="1">
+        <v>0</v>
+      </c>
       <c r="CL12" s="1"/>
-      <c r="CM12" s="1"/>
-      <c r="CN12" s="1"/>
+      <c r="CM12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CN12" s="1">
+        <v>0</v>
+      </c>
       <c r="CO12" s="1"/>
-      <c r="CP12" s="1"/>
-      <c r="CQ12" s="1"/>
+      <c r="CP12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CQ12" s="1">
+        <v>5</v>
+      </c>
       <c r="CR12" s="1"/>
-      <c r="CS12" s="1"/>
-      <c r="CT12" s="1"/>
+      <c r="CS12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CT12" s="1">
+        <v>1</v>
+      </c>
       <c r="CU12" s="1"/>
+      <c r="CV12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CW12" s="1">
+        <v>6</v>
+      </c>
+      <c r="CX12" s="1"/>
+      <c r="CY12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="CZ12" s="1">
+        <v>0</v>
+      </c>
+      <c r="DA12" s="1"/>
+      <c r="DB12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="DC12" s="1">
+        <v>9</v>
+      </c>
+      <c r="DD12" s="1"/>
+      <c r="DE12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="DF12" s="1">
+        <v>8</v>
+      </c>
+      <c r="DG12" s="1"/>
+      <c r="DH12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="DI12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DJ12" s="1"/>
+      <c r="DK12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="DL12" s="1">
+        <v>10</v>
+      </c>
+      <c r="DM12" s="1"/>
+      <c r="DN12" s="1">
+        <v>-10</v>
+      </c>
+      <c r="DO12" s="1">
+        <v>1</v>
+      </c>
+      <c r="DP12" s="1"/>
+      <c r="DQ12" s="1"/>
+      <c r="DR12" s="1"/>
+      <c r="DS12" s="1"/>
+      <c r="DT12" s="1"/>
+      <c r="DU12" s="1"/>
+      <c r="DV12" s="1"/>
+      <c r="DW12" s="1"/>
+      <c r="DX12" s="1"/>
+      <c r="DY12" s="1"/>
+      <c r="DZ12" s="1"/>
+      <c r="EA12" s="1"/>
+      <c r="EB12" s="1"/>
+      <c r="EC12" s="1"/>
+      <c r="ED12" s="1"/>
+      <c r="EE12" s="1"/>
+      <c r="EF12" s="1"/>
+      <c r="EG12" s="1"/>
+      <c r="EH12" s="1"/>
+      <c r="EI12" s="1"/>
+      <c r="EJ12" s="1"/>
+      <c r="EK12" s="1"/>
+      <c r="EL12" s="1"/>
+      <c r="EM12" s="1"/>
+      <c r="EN12" s="1"/>
+      <c r="EO12" s="1"/>
+      <c r="EP12" s="1"/>
+      <c r="EQ12" s="1"/>
+      <c r="ER12" s="1"/>
+      <c r="ES12" s="1"/>
+      <c r="ET12" s="1"/>
+      <c r="EU12" s="1"/>
+      <c r="EV12" s="1"/>
+      <c r="EW12" s="1"/>
+      <c r="EX12" s="1"/>
     </row>
-    <row r="13" spans="1:99" ht="15.75" customHeight="1">
+    <row r="13" spans="1:154" ht="15.75" customHeight="1">
       <c r="A13" s="1">
         <v>-9.5</v>
       </c>
@@ -3052,26 +4341,133 @@
         <v>4</v>
       </c>
       <c r="CC13" s="1"/>
-      <c r="CD13" s="1"/>
-      <c r="CE13" s="1"/>
+      <c r="CD13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CE13" s="1">
+        <v>4</v>
+      </c>
       <c r="CF13" s="1"/>
-      <c r="CG13" s="1"/>
-      <c r="CH13" s="1"/>
+      <c r="CG13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CH13" s="1">
+        <v>2</v>
+      </c>
       <c r="CI13" s="1"/>
-      <c r="CJ13" s="1"/>
-      <c r="CK13" s="1"/>
+      <c r="CJ13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CK13" s="1">
+        <v>0</v>
+      </c>
       <c r="CL13" s="1"/>
-      <c r="CM13" s="1"/>
-      <c r="CN13" s="1"/>
+      <c r="CM13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CN13" s="1">
+        <v>4</v>
+      </c>
       <c r="CO13" s="1"/>
-      <c r="CP13" s="1"/>
-      <c r="CQ13" s="1"/>
+      <c r="CP13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CQ13" s="1">
+        <v>11</v>
+      </c>
       <c r="CR13" s="1"/>
-      <c r="CS13" s="1"/>
-      <c r="CT13" s="1"/>
+      <c r="CS13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CT13" s="1">
+        <v>1</v>
+      </c>
       <c r="CU13" s="1"/>
+      <c r="CV13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CW13" s="1">
+        <v>6</v>
+      </c>
+      <c r="CX13" s="1"/>
+      <c r="CY13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="CZ13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DA13" s="1"/>
+      <c r="DB13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="DC13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD13" s="1"/>
+      <c r="DE13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="DF13" s="1">
+        <v>10</v>
+      </c>
+      <c r="DG13" s="1"/>
+      <c r="DH13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="DI13" s="1">
+        <v>4</v>
+      </c>
+      <c r="DJ13" s="1"/>
+      <c r="DK13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="DL13" s="1">
+        <v>5</v>
+      </c>
+      <c r="DM13" s="1"/>
+      <c r="DN13" s="1">
+        <v>-11</v>
+      </c>
+      <c r="DO13" s="1">
+        <v>3</v>
+      </c>
+      <c r="DP13" s="1"/>
+      <c r="DQ13" s="1"/>
+      <c r="DR13" s="1"/>
+      <c r="DS13" s="1"/>
+      <c r="DT13" s="1"/>
+      <c r="DU13" s="1"/>
+      <c r="DV13" s="1"/>
+      <c r="DW13" s="1"/>
+      <c r="DX13" s="1"/>
+      <c r="DY13" s="1"/>
+      <c r="DZ13" s="1"/>
+      <c r="EA13" s="1"/>
+      <c r="EB13" s="1"/>
+      <c r="EC13" s="1"/>
+      <c r="ED13" s="1"/>
+      <c r="EE13" s="1"/>
+      <c r="EF13" s="1"/>
+      <c r="EG13" s="1"/>
+      <c r="EH13" s="1"/>
+      <c r="EI13" s="1"/>
+      <c r="EJ13" s="1"/>
+      <c r="EK13" s="1"/>
+      <c r="EL13" s="1"/>
+      <c r="EM13" s="1"/>
+      <c r="EN13" s="1"/>
+      <c r="EO13" s="1"/>
+      <c r="EP13" s="1"/>
+      <c r="EQ13" s="1"/>
+      <c r="ER13" s="1"/>
+      <c r="ES13" s="1"/>
+      <c r="ET13" s="1"/>
+      <c r="EU13" s="1"/>
+      <c r="EV13" s="1"/>
+      <c r="EW13" s="1"/>
+      <c r="EX13" s="1"/>
     </row>
-    <row r="14" spans="1:99" ht="15.75" customHeight="1">
+    <row r="14" spans="1:154" ht="15.75" customHeight="1">
       <c r="A14" s="1">
         <v>-10</v>
       </c>
@@ -3253,26 +4649,133 @@
         <v>2</v>
       </c>
       <c r="CC14" s="1"/>
-      <c r="CD14" s="1"/>
-      <c r="CE14" s="1"/>
+      <c r="CD14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CE14" s="1">
+        <v>6</v>
+      </c>
       <c r="CF14" s="1"/>
-      <c r="CG14" s="1"/>
-      <c r="CH14" s="1"/>
+      <c r="CG14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CH14" s="1">
+        <v>2</v>
+      </c>
       <c r="CI14" s="1"/>
-      <c r="CJ14" s="1"/>
-      <c r="CK14" s="1"/>
+      <c r="CJ14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CK14" s="1">
+        <v>7</v>
+      </c>
       <c r="CL14" s="1"/>
-      <c r="CM14" s="1"/>
-      <c r="CN14" s="1"/>
+      <c r="CM14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CN14" s="1">
+        <v>4</v>
+      </c>
       <c r="CO14" s="1"/>
-      <c r="CP14" s="1"/>
-      <c r="CQ14" s="1"/>
+      <c r="CP14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CQ14" s="1">
+        <v>15</v>
+      </c>
       <c r="CR14" s="1"/>
-      <c r="CS14" s="1"/>
-      <c r="CT14" s="1"/>
+      <c r="CS14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CT14" s="1">
+        <v>4</v>
+      </c>
       <c r="CU14" s="1"/>
+      <c r="CV14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CW14" s="1">
+        <v>5</v>
+      </c>
+      <c r="CX14" s="1"/>
+      <c r="CY14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="CZ14" s="1">
+        <v>2</v>
+      </c>
+      <c r="DA14" s="1"/>
+      <c r="DB14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="DC14" s="1">
+        <v>15</v>
+      </c>
+      <c r="DD14" s="1"/>
+      <c r="DE14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="DF14" s="1">
+        <v>19</v>
+      </c>
+      <c r="DG14" s="1"/>
+      <c r="DH14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="DI14" s="1">
+        <v>5</v>
+      </c>
+      <c r="DJ14" s="1"/>
+      <c r="DK14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="DL14" s="1">
+        <v>13</v>
+      </c>
+      <c r="DM14" s="1"/>
+      <c r="DN14" s="1">
+        <v>-12</v>
+      </c>
+      <c r="DO14" s="1">
+        <v>0</v>
+      </c>
+      <c r="DP14" s="1"/>
+      <c r="DQ14" s="1"/>
+      <c r="DR14" s="1"/>
+      <c r="DS14" s="1"/>
+      <c r="DT14" s="1"/>
+      <c r="DU14" s="1"/>
+      <c r="DV14" s="1"/>
+      <c r="DW14" s="1"/>
+      <c r="DX14" s="1"/>
+      <c r="DY14" s="1"/>
+      <c r="DZ14" s="1"/>
+      <c r="EA14" s="1"/>
+      <c r="EB14" s="1"/>
+      <c r="EC14" s="1"/>
+      <c r="ED14" s="1"/>
+      <c r="EE14" s="1"/>
+      <c r="EF14" s="1"/>
+      <c r="EG14" s="1"/>
+      <c r="EH14" s="1"/>
+      <c r="EI14" s="1"/>
+      <c r="EJ14" s="1"/>
+      <c r="EK14" s="1"/>
+      <c r="EL14" s="1"/>
+      <c r="EM14" s="1"/>
+      <c r="EN14" s="1"/>
+      <c r="EO14" s="1"/>
+      <c r="EP14" s="1"/>
+      <c r="EQ14" s="1"/>
+      <c r="ER14" s="1"/>
+      <c r="ES14" s="1"/>
+      <c r="ET14" s="1"/>
+      <c r="EU14" s="1"/>
+      <c r="EV14" s="1"/>
+      <c r="EW14" s="1"/>
+      <c r="EX14" s="1"/>
     </row>
-    <row r="15" spans="1:99" ht="15.75" customHeight="1">
+    <row r="15" spans="1:154" ht="15.75" customHeight="1">
       <c r="A15" s="1">
         <v>-10.5</v>
       </c>
@@ -3454,26 +4957,133 @@
         <v>10</v>
       </c>
       <c r="CC15" s="1"/>
-      <c r="CD15" s="1"/>
-      <c r="CE15" s="1"/>
+      <c r="CD15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CE15" s="1">
+        <v>8</v>
+      </c>
       <c r="CF15" s="1"/>
-      <c r="CG15" s="1"/>
-      <c r="CH15" s="1"/>
+      <c r="CG15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CH15" s="1">
+        <v>2</v>
+      </c>
       <c r="CI15" s="1"/>
-      <c r="CJ15" s="1"/>
-      <c r="CK15" s="1"/>
+      <c r="CJ15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CK15" s="1">
+        <v>10</v>
+      </c>
       <c r="CL15" s="1"/>
-      <c r="CM15" s="1"/>
-      <c r="CN15" s="1"/>
+      <c r="CM15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CN15" s="1">
+        <v>7</v>
+      </c>
       <c r="CO15" s="1"/>
-      <c r="CP15" s="1"/>
-      <c r="CQ15" s="1"/>
+      <c r="CP15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CQ15" s="1">
+        <v>18</v>
+      </c>
       <c r="CR15" s="1"/>
-      <c r="CS15" s="1"/>
-      <c r="CT15" s="1"/>
+      <c r="CS15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CT15" s="1">
+        <v>3</v>
+      </c>
       <c r="CU15" s="1"/>
+      <c r="CV15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CW15" s="1">
+        <v>5</v>
+      </c>
+      <c r="CX15" s="1"/>
+      <c r="CY15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="CZ15" s="1">
+        <v>14</v>
+      </c>
+      <c r="DA15" s="1"/>
+      <c r="DB15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="DC15" s="1">
+        <v>21</v>
+      </c>
+      <c r="DD15" s="1"/>
+      <c r="DE15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="DF15" s="1">
+        <v>13</v>
+      </c>
+      <c r="DG15" s="1"/>
+      <c r="DH15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="DI15" s="1">
+        <v>3</v>
+      </c>
+      <c r="DJ15" s="1"/>
+      <c r="DK15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="DL15" s="1">
+        <v>12</v>
+      </c>
+      <c r="DM15" s="1"/>
+      <c r="DN15" s="1">
+        <v>-13</v>
+      </c>
+      <c r="DO15" s="1">
+        <v>6</v>
+      </c>
+      <c r="DP15" s="1"/>
+      <c r="DQ15" s="1"/>
+      <c r="DR15" s="1"/>
+      <c r="DS15" s="1"/>
+      <c r="DT15" s="1"/>
+      <c r="DU15" s="1"/>
+      <c r="DV15" s="1"/>
+      <c r="DW15" s="1"/>
+      <c r="DX15" s="1"/>
+      <c r="DY15" s="1"/>
+      <c r="DZ15" s="1"/>
+      <c r="EA15" s="1"/>
+      <c r="EB15" s="1"/>
+      <c r="EC15" s="1"/>
+      <c r="ED15" s="1"/>
+      <c r="EE15" s="1"/>
+      <c r="EF15" s="1"/>
+      <c r="EG15" s="1"/>
+      <c r="EH15" s="1"/>
+      <c r="EI15" s="1"/>
+      <c r="EJ15" s="1"/>
+      <c r="EK15" s="1"/>
+      <c r="EL15" s="1"/>
+      <c r="EM15" s="1"/>
+      <c r="EN15" s="1"/>
+      <c r="EO15" s="1"/>
+      <c r="EP15" s="1"/>
+      <c r="EQ15" s="1"/>
+      <c r="ER15" s="1"/>
+      <c r="ES15" s="1"/>
+      <c r="ET15" s="1"/>
+      <c r="EU15" s="1"/>
+      <c r="EV15" s="1"/>
+      <c r="EW15" s="1"/>
+      <c r="EX15" s="1"/>
     </row>
-    <row r="16" spans="1:99" ht="15.75" customHeight="1">
+    <row r="16" spans="1:154" ht="15.75" customHeight="1">
       <c r="A16" s="1">
         <v>-11</v>
       </c>
@@ -3655,26 +5265,133 @@
         <v>3</v>
       </c>
       <c r="CC16" s="1"/>
-      <c r="CD16" s="1"/>
-      <c r="CE16" s="1"/>
+      <c r="CD16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CE16" s="1">
+        <v>3</v>
+      </c>
       <c r="CF16" s="1"/>
-      <c r="CG16" s="1"/>
-      <c r="CH16" s="1"/>
+      <c r="CG16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CH16" s="1">
+        <v>4</v>
+      </c>
       <c r="CI16" s="1"/>
-      <c r="CJ16" s="1"/>
-      <c r="CK16" s="1"/>
+      <c r="CJ16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CK16" s="1">
+        <v>29</v>
+      </c>
       <c r="CL16" s="1"/>
-      <c r="CM16" s="1"/>
-      <c r="CN16" s="1"/>
+      <c r="CM16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CN16" s="1">
+        <v>15</v>
+      </c>
       <c r="CO16" s="1"/>
-      <c r="CP16" s="1"/>
-      <c r="CQ16" s="1"/>
+      <c r="CP16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CQ16" s="1">
+        <v>15</v>
+      </c>
       <c r="CR16" s="1"/>
-      <c r="CS16" s="1"/>
-      <c r="CT16" s="1"/>
+      <c r="CS16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CT16" s="1">
+        <v>6</v>
+      </c>
       <c r="CU16" s="1"/>
+      <c r="CV16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CW16" s="1">
+        <v>18</v>
+      </c>
+      <c r="CX16" s="1"/>
+      <c r="CY16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="CZ16" s="1">
+        <v>12</v>
+      </c>
+      <c r="DA16" s="1"/>
+      <c r="DB16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="DC16" s="1">
+        <v>24</v>
+      </c>
+      <c r="DD16" s="1"/>
+      <c r="DE16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="DF16" s="1">
+        <v>15</v>
+      </c>
+      <c r="DG16" s="1"/>
+      <c r="DH16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="DI16" s="1">
+        <v>15</v>
+      </c>
+      <c r="DJ16" s="1"/>
+      <c r="DK16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="DL16" s="1">
+        <v>7</v>
+      </c>
+      <c r="DM16" s="1"/>
+      <c r="DN16" s="1">
+        <v>-14</v>
+      </c>
+      <c r="DO16" s="1">
+        <v>5</v>
+      </c>
+      <c r="DP16" s="1"/>
+      <c r="DQ16" s="1"/>
+      <c r="DR16" s="1"/>
+      <c r="DS16" s="1"/>
+      <c r="DT16" s="1"/>
+      <c r="DU16" s="1"/>
+      <c r="DV16" s="1"/>
+      <c r="DW16" s="1"/>
+      <c r="DX16" s="1"/>
+      <c r="DY16" s="1"/>
+      <c r="DZ16" s="1"/>
+      <c r="EA16" s="1"/>
+      <c r="EB16" s="1"/>
+      <c r="EC16" s="1"/>
+      <c r="ED16" s="1"/>
+      <c r="EE16" s="1"/>
+      <c r="EF16" s="1"/>
+      <c r="EG16" s="1"/>
+      <c r="EH16" s="1"/>
+      <c r="EI16" s="1"/>
+      <c r="EJ16" s="1"/>
+      <c r="EK16" s="1"/>
+      <c r="EL16" s="1"/>
+      <c r="EM16" s="1"/>
+      <c r="EN16" s="1"/>
+      <c r="EO16" s="1"/>
+      <c r="EP16" s="1"/>
+      <c r="EQ16" s="1"/>
+      <c r="ER16" s="1"/>
+      <c r="ES16" s="1"/>
+      <c r="ET16" s="1"/>
+      <c r="EU16" s="1"/>
+      <c r="EV16" s="1"/>
+      <c r="EW16" s="1"/>
+      <c r="EX16" s="1"/>
     </row>
-    <row r="17" spans="1:99" ht="15.75" customHeight="1">
+    <row r="17" spans="1:154" ht="15.75" customHeight="1">
       <c r="A17" s="1">
         <v>-11.5</v>
       </c>
@@ -3856,26 +5573,133 @@
         <v>11</v>
       </c>
       <c r="CC17" s="1"/>
-      <c r="CD17" s="1"/>
-      <c r="CE17" s="1"/>
+      <c r="CD17" s="1">
+        <v>-15.5</v>
+      </c>
+      <c r="CE17" s="1">
+        <v>9</v>
+      </c>
       <c r="CF17" s="1"/>
-      <c r="CG17" s="1"/>
-      <c r="CH17" s="1"/>
+      <c r="CG17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CH17" s="1">
+        <v>11</v>
+      </c>
       <c r="CI17" s="1"/>
-      <c r="CJ17" s="1"/>
-      <c r="CK17" s="1"/>
+      <c r="CJ17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CK17" s="1">
+        <v>18</v>
+      </c>
       <c r="CL17" s="1"/>
-      <c r="CM17" s="1"/>
-      <c r="CN17" s="1"/>
+      <c r="CM17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CN17" s="1">
+        <v>15</v>
+      </c>
       <c r="CO17" s="1"/>
-      <c r="CP17" s="1"/>
-      <c r="CQ17" s="1"/>
+      <c r="CP17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CQ17" s="1">
+        <v>14</v>
+      </c>
       <c r="CR17" s="1"/>
-      <c r="CS17" s="1"/>
-      <c r="CT17" s="1"/>
+      <c r="CS17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CT17" s="1">
+        <v>6</v>
+      </c>
       <c r="CU17" s="1"/>
+      <c r="CV17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CW17" s="1">
+        <v>20</v>
+      </c>
+      <c r="CX17" s="1"/>
+      <c r="CY17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="CZ17" s="1">
+        <v>17</v>
+      </c>
+      <c r="DA17" s="1"/>
+      <c r="DB17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="DC17" s="1">
+        <v>9</v>
+      </c>
+      <c r="DD17" s="1"/>
+      <c r="DE17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="DF17" s="1">
+        <v>9</v>
+      </c>
+      <c r="DG17" s="1"/>
+      <c r="DH17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="DI17" s="1">
+        <v>19</v>
+      </c>
+      <c r="DJ17" s="1"/>
+      <c r="DK17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="DL17" s="1">
+        <v>6</v>
+      </c>
+      <c r="DM17" s="1"/>
+      <c r="DN17" s="1">
+        <v>-15</v>
+      </c>
+      <c r="DO17" s="1">
+        <v>12</v>
+      </c>
+      <c r="DP17" s="1"/>
+      <c r="DQ17" s="1"/>
+      <c r="DR17" s="1"/>
+      <c r="DS17" s="1"/>
+      <c r="DT17" s="1"/>
+      <c r="DU17" s="1"/>
+      <c r="DV17" s="1"/>
+      <c r="DW17" s="1"/>
+      <c r="DX17" s="1"/>
+      <c r="DY17" s="1"/>
+      <c r="DZ17" s="1"/>
+      <c r="EA17" s="1"/>
+      <c r="EB17" s="1"/>
+      <c r="EC17" s="1"/>
+      <c r="ED17" s="1"/>
+      <c r="EE17" s="1"/>
+      <c r="EF17" s="1"/>
+      <c r="EG17" s="1"/>
+      <c r="EH17" s="1"/>
+      <c r="EI17" s="1"/>
+      <c r="EJ17" s="1"/>
+      <c r="EK17" s="1"/>
+      <c r="EL17" s="1"/>
+      <c r="EM17" s="1"/>
+      <c r="EN17" s="1"/>
+      <c r="EO17" s="1"/>
+      <c r="EP17" s="1"/>
+      <c r="EQ17" s="1"/>
+      <c r="ER17" s="1"/>
+      <c r="ES17" s="1"/>
+      <c r="ET17" s="1"/>
+      <c r="EU17" s="1"/>
+      <c r="EV17" s="1"/>
+      <c r="EW17" s="1"/>
+      <c r="EX17" s="1"/>
     </row>
-    <row r="18" spans="1:99" ht="15.75" customHeight="1">
+    <row r="18" spans="1:154" ht="15.75" customHeight="1">
       <c r="A18" s="1">
         <v>-12</v>
       </c>
@@ -4057,26 +5881,133 @@
         <v>20</v>
       </c>
       <c r="CC18" s="1"/>
-      <c r="CD18" s="1"/>
-      <c r="CE18" s="1"/>
+      <c r="CD18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CE18" s="1">
+        <v>5</v>
+      </c>
       <c r="CF18" s="1"/>
-      <c r="CG18" s="1"/>
-      <c r="CH18" s="1"/>
+      <c r="CG18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CH18" s="1">
+        <v>7</v>
+      </c>
       <c r="CI18" s="1"/>
-      <c r="CJ18" s="1"/>
-      <c r="CK18" s="1"/>
+      <c r="CJ18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CK18" s="1">
+        <v>14</v>
+      </c>
       <c r="CL18" s="1"/>
-      <c r="CM18" s="1"/>
-      <c r="CN18" s="1"/>
+      <c r="CM18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CN18" s="1">
+        <v>20</v>
+      </c>
       <c r="CO18" s="1"/>
-      <c r="CP18" s="1"/>
-      <c r="CQ18" s="1"/>
+      <c r="CP18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CQ18" s="1">
+        <v>6</v>
+      </c>
       <c r="CR18" s="1"/>
-      <c r="CS18" s="1"/>
-      <c r="CT18" s="1"/>
+      <c r="CS18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CT18" s="1">
+        <v>11</v>
+      </c>
       <c r="CU18" s="1"/>
+      <c r="CV18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CW18" s="1">
+        <v>26</v>
+      </c>
+      <c r="CX18" s="1"/>
+      <c r="CY18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="CZ18" s="1">
+        <v>8</v>
+      </c>
+      <c r="DA18" s="1"/>
+      <c r="DB18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="DC18" s="1">
+        <v>4</v>
+      </c>
+      <c r="DD18" s="1"/>
+      <c r="DE18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="DF18" s="1">
+        <v>13</v>
+      </c>
+      <c r="DG18" s="1"/>
+      <c r="DH18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="DI18" s="1">
+        <v>20</v>
+      </c>
+      <c r="DJ18" s="1"/>
+      <c r="DK18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="DL18" s="1">
+        <v>6</v>
+      </c>
+      <c r="DM18" s="1"/>
+      <c r="DN18" s="1">
+        <v>-16</v>
+      </c>
+      <c r="DO18" s="1">
+        <v>24</v>
+      </c>
+      <c r="DP18" s="1"/>
+      <c r="DQ18" s="1"/>
+      <c r="DR18" s="1"/>
+      <c r="DS18" s="1"/>
+      <c r="DT18" s="1"/>
+      <c r="DU18" s="1"/>
+      <c r="DV18" s="1"/>
+      <c r="DW18" s="1"/>
+      <c r="DX18" s="1"/>
+      <c r="DY18" s="1"/>
+      <c r="DZ18" s="1"/>
+      <c r="EA18" s="1"/>
+      <c r="EB18" s="1"/>
+      <c r="EC18" s="1"/>
+      <c r="ED18" s="1"/>
+      <c r="EE18" s="1"/>
+      <c r="EF18" s="1"/>
+      <c r="EG18" s="1"/>
+      <c r="EH18" s="1"/>
+      <c r="EI18" s="1"/>
+      <c r="EJ18" s="1"/>
+      <c r="EK18" s="1"/>
+      <c r="EL18" s="1"/>
+      <c r="EM18" s="1"/>
+      <c r="EN18" s="1"/>
+      <c r="EO18" s="1"/>
+      <c r="EP18" s="1"/>
+      <c r="EQ18" s="1"/>
+      <c r="ER18" s="1"/>
+      <c r="ES18" s="1"/>
+      <c r="ET18" s="1"/>
+      <c r="EU18" s="1"/>
+      <c r="EV18" s="1"/>
+      <c r="EW18" s="1"/>
+      <c r="EX18" s="1"/>
     </row>
-    <row r="19" spans="1:99" ht="15.75" customHeight="1">
+    <row r="19" spans="1:154" ht="15.75" customHeight="1">
       <c r="A19" s="1">
         <v>-12.5</v>
       </c>
@@ -4258,26 +6189,133 @@
         <v>12</v>
       </c>
       <c r="CC19" s="1"/>
-      <c r="CD19" s="1"/>
-      <c r="CE19" s="1"/>
+      <c r="CD19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CE19" s="1">
+        <v>16</v>
+      </c>
       <c r="CF19" s="1"/>
-      <c r="CG19" s="1"/>
-      <c r="CH19" s="1"/>
+      <c r="CG19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CH19" s="1">
+        <v>6</v>
+      </c>
       <c r="CI19" s="1"/>
-      <c r="CJ19" s="1"/>
-      <c r="CK19" s="1"/>
+      <c r="CJ19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CK19" s="1">
+        <v>12</v>
+      </c>
       <c r="CL19" s="1"/>
-      <c r="CM19" s="1"/>
-      <c r="CN19" s="1"/>
+      <c r="CM19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CN19" s="1">
+        <v>21</v>
+      </c>
       <c r="CO19" s="1"/>
-      <c r="CP19" s="1"/>
-      <c r="CQ19" s="1"/>
+      <c r="CP19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CQ19" s="1">
+        <v>5</v>
+      </c>
       <c r="CR19" s="1"/>
-      <c r="CS19" s="1"/>
-      <c r="CT19" s="1"/>
+      <c r="CS19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CT19" s="1">
+        <v>2</v>
+      </c>
       <c r="CU19" s="1"/>
+      <c r="CV19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CW19" s="1">
+        <v>5</v>
+      </c>
+      <c r="CX19" s="1"/>
+      <c r="CY19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="CZ19" s="1">
+        <v>15</v>
+      </c>
+      <c r="DA19" s="1"/>
+      <c r="DB19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="DC19" s="1">
+        <v>0</v>
+      </c>
+      <c r="DD19" s="1"/>
+      <c r="DE19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="DF19" s="1">
+        <v>3</v>
+      </c>
+      <c r="DG19" s="1"/>
+      <c r="DH19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="DI19" s="1">
+        <v>19</v>
+      </c>
+      <c r="DJ19" s="1"/>
+      <c r="DK19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="DL19" s="1">
+        <v>6</v>
+      </c>
+      <c r="DM19" s="1"/>
+      <c r="DN19" s="1">
+        <v>-17</v>
+      </c>
+      <c r="DO19" s="1">
+        <v>19</v>
+      </c>
+      <c r="DP19" s="1"/>
+      <c r="DQ19" s="1"/>
+      <c r="DR19" s="1"/>
+      <c r="DS19" s="1"/>
+      <c r="DT19" s="1"/>
+      <c r="DU19" s="1"/>
+      <c r="DV19" s="1"/>
+      <c r="DW19" s="1"/>
+      <c r="DX19" s="1"/>
+      <c r="DY19" s="1"/>
+      <c r="DZ19" s="1"/>
+      <c r="EA19" s="1"/>
+      <c r="EB19" s="1"/>
+      <c r="EC19" s="1"/>
+      <c r="ED19" s="1"/>
+      <c r="EE19" s="1"/>
+      <c r="EF19" s="1"/>
+      <c r="EG19" s="1"/>
+      <c r="EH19" s="1"/>
+      <c r="EI19" s="1"/>
+      <c r="EJ19" s="1"/>
+      <c r="EK19" s="1"/>
+      <c r="EL19" s="1"/>
+      <c r="EM19" s="1"/>
+      <c r="EN19" s="1"/>
+      <c r="EO19" s="1"/>
+      <c r="EP19" s="1"/>
+      <c r="EQ19" s="1"/>
+      <c r="ER19" s="1"/>
+      <c r="ES19" s="1"/>
+      <c r="ET19" s="1"/>
+      <c r="EU19" s="1"/>
+      <c r="EV19" s="1"/>
+      <c r="EW19" s="1"/>
+      <c r="EX19" s="1"/>
     </row>
-    <row r="20" spans="1:99" ht="15.75" customHeight="1">
+    <row r="20" spans="1:154" ht="15.75" customHeight="1">
       <c r="A20" s="1">
         <v>-13</v>
       </c>
@@ -4448,26 +6486,133 @@
         <v>9</v>
       </c>
       <c r="CC20" s="1"/>
-      <c r="CD20" s="1"/>
-      <c r="CE20" s="1"/>
+      <c r="CD20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CE20" s="1">
+        <v>7</v>
+      </c>
       <c r="CF20" s="1"/>
-      <c r="CG20" s="1"/>
-      <c r="CH20" s="1"/>
+      <c r="CG20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CH20" s="1">
+        <v>17</v>
+      </c>
       <c r="CI20" s="1"/>
-      <c r="CJ20" s="1"/>
-      <c r="CK20" s="1"/>
+      <c r="CJ20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CK20" s="1">
+        <v>8</v>
+      </c>
       <c r="CL20" s="1"/>
-      <c r="CM20" s="1"/>
-      <c r="CN20" s="1"/>
+      <c r="CM20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CN20" s="1">
+        <v>11</v>
+      </c>
       <c r="CO20" s="1"/>
-      <c r="CP20" s="1"/>
-      <c r="CQ20" s="1"/>
+      <c r="CP20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CQ20" s="1">
+        <v>5</v>
+      </c>
       <c r="CR20" s="1"/>
-      <c r="CS20" s="1"/>
-      <c r="CT20" s="1"/>
+      <c r="CS20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CT20" s="1">
+        <v>10</v>
+      </c>
       <c r="CU20" s="1"/>
+      <c r="CV20" s="1">
+        <v>-17.5</v>
+      </c>
+      <c r="CW20" s="1">
+        <v>2</v>
+      </c>
+      <c r="CX20" s="1"/>
+      <c r="CY20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="CZ20" s="1">
+        <v>12</v>
+      </c>
+      <c r="DA20" s="1"/>
+      <c r="DB20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="DC20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD20" s="1"/>
+      <c r="DE20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="DF20" s="1">
+        <v>1</v>
+      </c>
+      <c r="DG20" s="1"/>
+      <c r="DH20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="DI20" s="1">
+        <v>10</v>
+      </c>
+      <c r="DJ20" s="1"/>
+      <c r="DK20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="DL20" s="1">
+        <v>4</v>
+      </c>
+      <c r="DM20" s="1"/>
+      <c r="DN20" s="1">
+        <v>-18</v>
+      </c>
+      <c r="DO20" s="1">
+        <v>26</v>
+      </c>
+      <c r="DP20" s="1"/>
+      <c r="DQ20" s="1"/>
+      <c r="DR20" s="1"/>
+      <c r="DS20" s="1"/>
+      <c r="DT20" s="1"/>
+      <c r="DU20" s="1"/>
+      <c r="DV20" s="1"/>
+      <c r="DW20" s="1"/>
+      <c r="DX20" s="1"/>
+      <c r="DY20" s="1"/>
+      <c r="DZ20" s="1"/>
+      <c r="EA20" s="1"/>
+      <c r="EB20" s="1"/>
+      <c r="EC20" s="1"/>
+      <c r="ED20" s="1"/>
+      <c r="EE20" s="1"/>
+      <c r="EF20" s="1"/>
+      <c r="EG20" s="1"/>
+      <c r="EH20" s="1"/>
+      <c r="EI20" s="1"/>
+      <c r="EJ20" s="1"/>
+      <c r="EK20" s="1"/>
+      <c r="EL20" s="1"/>
+      <c r="EM20" s="1"/>
+      <c r="EN20" s="1"/>
+      <c r="EO20" s="1"/>
+      <c r="EP20" s="1"/>
+      <c r="EQ20" s="1"/>
+      <c r="ER20" s="1"/>
+      <c r="ES20" s="1"/>
+      <c r="ET20" s="1"/>
+      <c r="EU20" s="1"/>
+      <c r="EV20" s="1"/>
+      <c r="EW20" s="1"/>
+      <c r="EX20" s="1"/>
     </row>
-    <row r="21" spans="1:99" ht="15.75" customHeight="1">
+    <row r="21" spans="1:154" ht="15.75" customHeight="1">
       <c r="A21" s="1">
         <v>-13.5</v>
       </c>
@@ -4612,26 +6757,129 @@
         <v>18</v>
       </c>
       <c r="CC21" s="1"/>
-      <c r="CD21" s="1"/>
-      <c r="CE21" s="1"/>
+      <c r="CD21" s="1">
+        <v>-18.5</v>
+      </c>
+      <c r="CE21" s="1">
+        <v>7</v>
+      </c>
       <c r="CF21" s="1"/>
-      <c r="CG21" s="1"/>
-      <c r="CH21" s="1"/>
+      <c r="CG21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CH21" s="1">
+        <v>12</v>
+      </c>
       <c r="CI21" s="1"/>
-      <c r="CJ21" s="1"/>
-      <c r="CK21" s="1"/>
+      <c r="CJ21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CK21" s="1">
+        <v>3</v>
+      </c>
       <c r="CL21" s="1"/>
-      <c r="CM21" s="1"/>
-      <c r="CN21" s="1"/>
+      <c r="CM21" s="1">
+        <v>-18.5</v>
+      </c>
+      <c r="CN21" s="1">
+        <v>1</v>
+      </c>
       <c r="CO21" s="1"/>
-      <c r="CP21" s="1"/>
-      <c r="CQ21" s="1"/>
+      <c r="CP21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CQ21" s="1">
+        <v>2</v>
+      </c>
       <c r="CR21" s="1"/>
-      <c r="CS21" s="1"/>
-      <c r="CT21" s="1"/>
+      <c r="CS21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CT21" s="1">
+        <v>15</v>
+      </c>
       <c r="CU21" s="1"/>
+      <c r="CV21" s="1"/>
+      <c r="CW21" s="1"/>
+      <c r="CX21" s="1"/>
+      <c r="CY21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CZ21" s="1">
+        <v>7</v>
+      </c>
+      <c r="DA21" s="1"/>
+      <c r="DB21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="DC21" s="1">
+        <v>1</v>
+      </c>
+      <c r="DD21" s="1"/>
+      <c r="DE21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="DF21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DG21" s="1"/>
+      <c r="DH21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="DI21" s="1">
+        <v>6</v>
+      </c>
+      <c r="DJ21" s="1"/>
+      <c r="DK21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="DL21" s="1">
+        <v>4</v>
+      </c>
+      <c r="DM21" s="1"/>
+      <c r="DN21" s="1">
+        <v>-19</v>
+      </c>
+      <c r="DO21" s="1">
+        <v>5</v>
+      </c>
+      <c r="DP21" s="1"/>
+      <c r="DQ21" s="1"/>
+      <c r="DR21" s="1"/>
+      <c r="DS21" s="1"/>
+      <c r="DT21" s="1"/>
+      <c r="DU21" s="1"/>
+      <c r="DV21" s="1"/>
+      <c r="DW21" s="1"/>
+      <c r="DX21" s="1"/>
+      <c r="DY21" s="1"/>
+      <c r="DZ21" s="1"/>
+      <c r="EA21" s="1"/>
+      <c r="EB21" s="1"/>
+      <c r="EC21" s="1"/>
+      <c r="ED21" s="1"/>
+      <c r="EE21" s="1"/>
+      <c r="EF21" s="1"/>
+      <c r="EG21" s="1"/>
+      <c r="EH21" s="1"/>
+      <c r="EI21" s="1"/>
+      <c r="EJ21" s="1"/>
+      <c r="EK21" s="1"/>
+      <c r="EL21" s="1"/>
+      <c r="EM21" s="1"/>
+      <c r="EN21" s="1"/>
+      <c r="EO21" s="1"/>
+      <c r="EP21" s="1"/>
+      <c r="EQ21" s="1"/>
+      <c r="ER21" s="1"/>
+      <c r="ES21" s="1"/>
+      <c r="ET21" s="1"/>
+      <c r="EU21" s="1"/>
+      <c r="EV21" s="1"/>
+      <c r="EW21" s="1"/>
+      <c r="EX21" s="1"/>
     </row>
-    <row r="22" spans="1:99" ht="15.75" customHeight="1">
+    <row r="22" spans="1:154" ht="15.75" customHeight="1">
       <c r="A22" s="1">
         <v>-14</v>
       </c>
@@ -4766,11 +7014,19 @@
         <v>5</v>
       </c>
       <c r="CC22" s="1"/>
-      <c r="CD22" s="1"/>
-      <c r="CE22" s="1"/>
+      <c r="CD22" s="1">
+        <v>-19</v>
+      </c>
+      <c r="CE22" s="1">
+        <v>3</v>
+      </c>
       <c r="CF22" s="1"/>
-      <c r="CG22" s="1"/>
-      <c r="CH22" s="1"/>
+      <c r="CG22" s="1">
+        <v>-20</v>
+      </c>
+      <c r="CH22" s="1">
+        <v>16</v>
+      </c>
       <c r="CI22" s="1"/>
       <c r="CJ22" s="1"/>
       <c r="CK22" s="1"/>
@@ -4781,11 +7037,73 @@
       <c r="CP22" s="1"/>
       <c r="CQ22" s="1"/>
       <c r="CR22" s="1"/>
-      <c r="CS22" s="1"/>
-      <c r="CT22" s="1"/>
+      <c r="CS22" s="1">
+        <v>-20</v>
+      </c>
+      <c r="CT22" s="1">
+        <v>11</v>
+      </c>
       <c r="CU22" s="1"/>
+      <c r="CV22" s="1"/>
+      <c r="CW22" s="1"/>
+      <c r="CX22" s="1"/>
+      <c r="CY22" s="1">
+        <v>-20</v>
+      </c>
+      <c r="CZ22" s="1">
+        <v>6</v>
+      </c>
+      <c r="DA22" s="1"/>
+      <c r="DB22" s="1"/>
+      <c r="DC22" s="1"/>
+      <c r="DD22" s="1"/>
+      <c r="DE22" s="1"/>
+      <c r="DG22" s="1"/>
+      <c r="DH22" s="1"/>
+      <c r="DI22" s="1"/>
+      <c r="DJ22" s="1"/>
+      <c r="DK22" s="1"/>
+      <c r="DL22" s="1"/>
+      <c r="DM22" s="1"/>
+      <c r="DN22" s="1"/>
+      <c r="DO22" s="1"/>
+      <c r="DP22" s="1"/>
+      <c r="DQ22" s="1"/>
+      <c r="DR22" s="1"/>
+      <c r="DS22" s="1"/>
+      <c r="DT22" s="1"/>
+      <c r="DU22" s="1"/>
+      <c r="DV22" s="1"/>
+      <c r="DW22" s="1"/>
+      <c r="DX22" s="1"/>
+      <c r="DY22" s="1"/>
+      <c r="DZ22" s="1"/>
+      <c r="EA22" s="1"/>
+      <c r="EB22" s="1"/>
+      <c r="EC22" s="1"/>
+      <c r="ED22" s="1"/>
+      <c r="EE22" s="1"/>
+      <c r="EF22" s="1"/>
+      <c r="EG22" s="1"/>
+      <c r="EH22" s="1"/>
+      <c r="EI22" s="1"/>
+      <c r="EJ22" s="1"/>
+      <c r="EK22" s="1"/>
+      <c r="EL22" s="1"/>
+      <c r="EM22" s="1"/>
+      <c r="EN22" s="1"/>
+      <c r="EO22" s="1"/>
+      <c r="EP22" s="1"/>
+      <c r="EQ22" s="1"/>
+      <c r="ER22" s="1"/>
+      <c r="ES22" s="1"/>
+      <c r="ET22" s="1"/>
+      <c r="EU22" s="1"/>
+      <c r="EV22" s="1"/>
+      <c r="EW22" s="1"/>
+      <c r="EX22" s="1"/>
     </row>
-    <row r="23" spans="1:99" ht="15.75" customHeight="1">
+    <row r="23" spans="1:154" ht="15.75" customHeight="1">
       <c r="A23" s="1">
         <v>-14.5</v>
       </c>
@@ -4912,11 +7230,19 @@
         <v>4</v>
       </c>
       <c r="CC23" s="1"/>
-      <c r="CD23" s="1"/>
-      <c r="CE23" s="1"/>
+      <c r="CD23" s="1">
+        <v>-19.5</v>
+      </c>
+      <c r="CE23" s="1">
+        <v>8</v>
+      </c>
       <c r="CF23" s="1"/>
-      <c r="CG23" s="1"/>
-      <c r="CH23" s="1"/>
+      <c r="CG23" s="1">
+        <v>-21</v>
+      </c>
+      <c r="CH23" s="1">
+        <v>12</v>
+      </c>
       <c r="CI23" s="1"/>
       <c r="CJ23" s="1"/>
       <c r="CK23" s="1"/>
@@ -4927,11 +7253,74 @@
       <c r="CP23" s="1"/>
       <c r="CQ23" s="1"/>
       <c r="CR23" s="1"/>
-      <c r="CS23" s="1"/>
-      <c r="CT23" s="1"/>
+      <c r="CS23" s="1">
+        <v>-21</v>
+      </c>
+      <c r="CT23" s="1">
+        <v>15</v>
+      </c>
       <c r="CU23" s="1"/>
+      <c r="CV23" s="1"/>
+      <c r="CW23" s="1"/>
+      <c r="CX23" s="1"/>
+      <c r="CY23" s="1">
+        <v>-21</v>
+      </c>
+      <c r="CZ23" s="1">
+        <v>2</v>
+      </c>
+      <c r="DA23" s="1"/>
+      <c r="DB23" s="1"/>
+      <c r="DC23" s="1"/>
+      <c r="DD23" s="1"/>
+      <c r="DE23" s="1"/>
+      <c r="DF23" s="1"/>
+      <c r="DG23" s="1"/>
+      <c r="DH23" s="1"/>
+      <c r="DI23" s="1"/>
+      <c r="DJ23" s="1"/>
+      <c r="DK23" s="1"/>
+      <c r="DL23" s="1"/>
+      <c r="DM23" s="1"/>
+      <c r="DN23" s="1"/>
+      <c r="DO23" s="1"/>
+      <c r="DP23" s="1"/>
+      <c r="DQ23" s="1"/>
+      <c r="DR23" s="1"/>
+      <c r="DS23" s="1"/>
+      <c r="DT23" s="1"/>
+      <c r="DU23" s="1"/>
+      <c r="DV23" s="1"/>
+      <c r="DW23" s="1"/>
+      <c r="DX23" s="1"/>
+      <c r="DY23" s="1"/>
+      <c r="DZ23" s="1"/>
+      <c r="EA23" s="1"/>
+      <c r="EB23" s="1"/>
+      <c r="EC23" s="1"/>
+      <c r="ED23" s="1"/>
+      <c r="EE23" s="1"/>
+      <c r="EF23" s="1"/>
+      <c r="EG23" s="1"/>
+      <c r="EH23" s="1"/>
+      <c r="EI23" s="1"/>
+      <c r="EJ23" s="1"/>
+      <c r="EK23" s="1"/>
+      <c r="EL23" s="1"/>
+      <c r="EM23" s="1"/>
+      <c r="EN23" s="1"/>
+      <c r="EO23" s="1"/>
+      <c r="EP23" s="1"/>
+      <c r="EQ23" s="1"/>
+      <c r="ER23" s="1"/>
+      <c r="ES23" s="1"/>
+      <c r="ET23" s="1"/>
+      <c r="EU23" s="1"/>
+      <c r="EV23" s="1"/>
+      <c r="EW23" s="1"/>
+      <c r="EX23" s="1"/>
     </row>
-    <row r="24" spans="1:99" ht="15.75" customHeight="1">
+    <row r="24" spans="1:154" ht="15.75" customHeight="1">
       <c r="A24" s="1">
         <v>-15</v>
       </c>
@@ -5035,11 +7424,19 @@
       <c r="CA24" s="1"/>
       <c r="CB24" s="1"/>
       <c r="CC24" s="1"/>
-      <c r="CD24" s="1"/>
-      <c r="CE24" s="1"/>
+      <c r="CD24" s="1">
+        <v>-20</v>
+      </c>
+      <c r="CE24" s="1">
+        <v>3</v>
+      </c>
       <c r="CF24" s="1"/>
-      <c r="CG24" s="1"/>
-      <c r="CH24" s="1"/>
+      <c r="CG24" s="1">
+        <v>-22</v>
+      </c>
+      <c r="CH24" s="1">
+        <v>6</v>
+      </c>
       <c r="CI24" s="1"/>
       <c r="CJ24" s="1"/>
       <c r="CK24" s="1"/>
@@ -5050,11 +7447,70 @@
       <c r="CP24" s="1"/>
       <c r="CQ24" s="1"/>
       <c r="CR24" s="1"/>
-      <c r="CS24" s="1"/>
-      <c r="CT24" s="1"/>
+      <c r="CS24" s="1">
+        <v>-22</v>
+      </c>
+      <c r="CT24" s="1">
+        <v>10</v>
+      </c>
       <c r="CU24" s="1"/>
+      <c r="CV24" s="1"/>
+      <c r="CW24" s="1"/>
+      <c r="CX24" s="1"/>
+      <c r="CY24" s="1"/>
+      <c r="CZ24" s="1"/>
+      <c r="DA24" s="1"/>
+      <c r="DB24" s="1"/>
+      <c r="DC24" s="1"/>
+      <c r="DD24" s="1"/>
+      <c r="DE24" s="1"/>
+      <c r="DF24" s="1"/>
+      <c r="DG24" s="1"/>
+      <c r="DH24" s="1"/>
+      <c r="DI24" s="1"/>
+      <c r="DJ24" s="1"/>
+      <c r="DK24" s="1"/>
+      <c r="DL24" s="1"/>
+      <c r="DM24" s="1"/>
+      <c r="DN24" s="1"/>
+      <c r="DO24" s="1"/>
+      <c r="DP24" s="1"/>
+      <c r="DQ24" s="1"/>
+      <c r="DR24" s="1"/>
+      <c r="DS24" s="1"/>
+      <c r="DT24" s="1"/>
+      <c r="DU24" s="1"/>
+      <c r="DV24" s="1"/>
+      <c r="DW24" s="1"/>
+      <c r="DX24" s="1"/>
+      <c r="DY24" s="1"/>
+      <c r="DZ24" s="1"/>
+      <c r="EA24" s="1"/>
+      <c r="EB24" s="1"/>
+      <c r="EC24" s="1"/>
+      <c r="ED24" s="1"/>
+      <c r="EE24" s="1"/>
+      <c r="EF24" s="1"/>
+      <c r="EG24" s="1"/>
+      <c r="EH24" s="1"/>
+      <c r="EI24" s="1"/>
+      <c r="EJ24" s="1"/>
+      <c r="EK24" s="1"/>
+      <c r="EL24" s="1"/>
+      <c r="EM24" s="1"/>
+      <c r="EN24" s="1"/>
+      <c r="EO24" s="1"/>
+      <c r="EP24" s="1"/>
+      <c r="EQ24" s="1"/>
+      <c r="ER24" s="1"/>
+      <c r="ES24" s="1"/>
+      <c r="ET24" s="1"/>
+      <c r="EU24" s="1"/>
+      <c r="EV24" s="1"/>
+      <c r="EW24" s="1"/>
+      <c r="EX24" s="1"/>
     </row>
-    <row r="25" spans="1:99" ht="15.75" customHeight="1">
+    <row r="25" spans="1:154" ht="15.75" customHeight="1">
       <c r="A25" s="1">
         <v>-15.5</v>
       </c>
@@ -5101,8 +7557,28 @@
       </c>
       <c r="CA25" s="1"/>
       <c r="CB25" s="1"/>
+      <c r="CD25" s="1">
+        <v>-21</v>
+      </c>
+      <c r="CE25" s="1">
+        <v>9</v>
+      </c>
+      <c r="CG25" s="1">
+        <v>-22.5</v>
+      </c>
+      <c r="CH25" s="1">
+        <v>1</v>
+      </c>
+      <c r="CS25" s="1">
+        <v>-23</v>
+      </c>
+      <c r="CT25" s="1">
+        <v>7</v>
+      </c>
+      <c r="CV25" s="1"/>
+      <c r="CW25" s="1"/>
     </row>
-    <row r="26" spans="1:99" ht="15.75" customHeight="1">
+    <row r="26" spans="1:154" ht="15.75" customHeight="1">
       <c r="A26" s="1">
         <v>-16</v>
       </c>
@@ -5121,8 +7597,20 @@
       <c r="N26" s="1">
         <v>4</v>
       </c>
+      <c r="CD26" s="1">
+        <v>-21.5</v>
+      </c>
+      <c r="CE26" s="1">
+        <v>4</v>
+      </c>
+      <c r="CG26" s="1">
+        <v>-23</v>
+      </c>
+      <c r="CH26" s="1">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:99" ht="15.75" customHeight="1">
+    <row r="27" spans="1:154" ht="15.75" customHeight="1">
       <c r="A27" s="1">
         <v>-16.5</v>
       </c>
@@ -5136,7 +7624,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:99" ht="15.75" customHeight="1">
+    <row r="28" spans="1:154" ht="15.75" customHeight="1">
       <c r="A28" s="1">
         <v>-17</v>
       </c>
@@ -5150,7 +7638,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:99" ht="15.75" customHeight="1">
+    <row r="29" spans="1:154" ht="15.75" customHeight="1">
       <c r="A29" s="1">
         <v>-17.5</v>
       </c>
@@ -5164,7 +7652,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:99" ht="15.75" customHeight="1">
+    <row r="30" spans="1:154" ht="15.75" customHeight="1">
       <c r="A30" s="1">
         <v>-18.5</v>
       </c>
@@ -5178,7 +7666,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:99" ht="15.75" customHeight="1">
+    <row r="31" spans="1:154" ht="15.75" customHeight="1">
       <c r="B31" s="1"/>
       <c r="J31" s="1">
         <v>-19</v>
@@ -5187,7 +7675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:99" ht="15.75" customHeight="1">
+    <row r="32" spans="1:154" ht="15.75" customHeight="1">
       <c r="J32" s="1">
         <v>-19.5</v>
       </c>

</xml_diff>